<commit_message>
Made new script for limited 14C runs. General scheme for everything is set.
</commit_message>
<xml_diff>
--- a/data/combined_14Clocations-edits.xlsx
+++ b/data/combined_14Clocations-edits.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/christopherkiahtipes/Dropbox/Temporary/2023_UGhent_Talk/Mapping_Bantu/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C65062DD-CD1B-6341-8638-31C393CC3A21}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{18F6D2DB-D3CD-2146-B7C8-CBF0A58879B6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="34180" yWindow="500" windowWidth="28040" windowHeight="17260" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="36700" yWindow="500" windowWidth="28040" windowHeight="17260" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="combined_14Clocations-edits" sheetId="1" r:id="rId1"/>
@@ -1316,7 +1316,7 @@
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="42">
+  <cellXfs count="43">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
@@ -1403,6 +1403,9 @@
     </xf>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="18" fillId="33" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="33" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="43">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -6350,8 +6353,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:F50"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="J23" sqref="J23"/>
+    <sheetView topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="G36" sqref="G36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -7375,17 +7378,17 @@
   <dimension ref="A1:M38"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F17" sqref="F17"/>
+      <selection activeCell="I8" sqref="I8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="19.6640625" customWidth="1"/>
     <col min="2" max="2" width="18" customWidth="1"/>
-    <col min="5" max="5" width="24.5" customWidth="1"/>
-    <col min="7" max="7" width="15.1640625" customWidth="1"/>
-    <col min="10" max="10" width="21" customWidth="1"/>
-    <col min="11" max="11" width="17.33203125" customWidth="1"/>
+    <col min="3" max="3" width="24.5" customWidth="1"/>
+    <col min="4" max="4" width="17.33203125" customWidth="1"/>
+    <col min="6" max="6" width="15.1640625" customWidth="1"/>
+    <col min="11" max="11" width="21" customWidth="1"/>
     <col min="12" max="12" width="9.33203125" customWidth="1"/>
     <col min="13" max="13" width="43.33203125" customWidth="1"/>
   </cols>
@@ -7398,31 +7401,31 @@
         <v>190</v>
       </c>
       <c r="C1" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="D1" s="6" t="s">
+        <v>188</v>
+      </c>
+      <c r="E1" s="6" t="s">
+        <v>229</v>
+      </c>
+      <c r="F1" s="6" t="s">
+        <v>230</v>
+      </c>
+      <c r="G1" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="D1" s="6" t="s">
+      <c r="H1" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="E1" s="6" t="s">
-        <v>36</v>
-      </c>
-      <c r="F1" s="6" t="s">
-        <v>229</v>
-      </c>
-      <c r="G1" s="6" t="s">
-        <v>230</v>
-      </c>
-      <c r="H1" s="6" t="s">
+      <c r="I1" s="6" t="s">
         <v>42</v>
       </c>
-      <c r="I1" s="6" t="s">
+      <c r="J1" s="6" t="s">
         <v>43</v>
       </c>
-      <c r="J1" s="6" t="s">
+      <c r="K1" s="6" t="s">
         <v>218</v>
-      </c>
-      <c r="K1" s="6" t="s">
-        <v>188</v>
       </c>
       <c r="L1" s="8" t="s">
         <v>187</v>
@@ -7435,35 +7438,35 @@
       <c r="A2" s="12" t="s">
         <v>132</v>
       </c>
-      <c r="B2" s="36" t="s">
+      <c r="B2" s="4" t="s">
         <v>74</v>
       </c>
-      <c r="C2" s="37">
+      <c r="C2" s="36" t="s">
+        <v>73</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>189</v>
+      </c>
+      <c r="E2" s="39">
+        <v>101</v>
+      </c>
+      <c r="F2" s="39" t="s">
+        <v>41</v>
+      </c>
+      <c r="G2" s="37">
         <v>6.4333330000000002</v>
       </c>
-      <c r="D2" s="37">
+      <c r="H2" s="37">
         <v>4.55</v>
       </c>
-      <c r="E2" s="36" t="s">
-        <v>73</v>
-      </c>
-      <c r="F2" s="39">
-        <v>101</v>
-      </c>
-      <c r="G2" s="39" t="s">
-        <v>41</v>
-      </c>
-      <c r="H2" s="36" t="s">
+      <c r="I2" s="36" t="s">
         <v>75</v>
       </c>
-      <c r="I2" s="36" t="s">
+      <c r="J2" s="36" t="s">
         <v>180</v>
       </c>
-      <c r="J2" s="36" t="s">
+      <c r="K2" s="36" t="s">
         <v>219</v>
-      </c>
-      <c r="K2" s="36" t="s">
-        <v>189</v>
       </c>
       <c r="L2" s="2"/>
       <c r="M2" s="2" t="s">
@@ -7474,35 +7477,35 @@
       <c r="A3" s="12" t="s">
         <v>125</v>
       </c>
-      <c r="B3" s="36" t="s">
+      <c r="B3" s="4" t="s">
         <v>106</v>
       </c>
-      <c r="C3" s="37">
+      <c r="C3" s="36" t="s">
+        <v>105</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>217</v>
+      </c>
+      <c r="E3" s="39">
+        <v>156</v>
+      </c>
+      <c r="F3" s="39" t="s">
+        <v>41</v>
+      </c>
+      <c r="G3" s="37">
         <v>10.4</v>
       </c>
-      <c r="D3" s="37">
+      <c r="H3" s="37">
         <v>2.39</v>
       </c>
-      <c r="E3" s="36" t="s">
-        <v>105</v>
-      </c>
-      <c r="F3" s="39">
-        <v>156</v>
-      </c>
-      <c r="G3" s="39" t="s">
-        <v>41</v>
-      </c>
-      <c r="H3" s="36" t="s">
+      <c r="I3" s="36" t="s">
         <v>65</v>
       </c>
-      <c r="I3" s="36" t="s">
+      <c r="J3" s="36" t="s">
         <v>180</v>
       </c>
-      <c r="J3" s="36" t="s">
+      <c r="K3" s="36" t="s">
         <v>223</v>
-      </c>
-      <c r="K3" s="36" t="s">
-        <v>217</v>
       </c>
       <c r="L3" s="2"/>
       <c r="M3" s="2" t="s">
@@ -7513,35 +7516,35 @@
       <c r="A4" s="30" t="s">
         <v>130</v>
       </c>
-      <c r="B4" s="36" t="s">
+      <c r="B4" s="4" t="s">
         <v>62</v>
       </c>
-      <c r="C4" s="37">
+      <c r="C4" s="36" t="s">
+        <v>61</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>189</v>
+      </c>
+      <c r="E4" s="39">
+        <v>242</v>
+      </c>
+      <c r="F4" s="39" t="s">
+        <v>41</v>
+      </c>
+      <c r="G4" s="37">
         <v>9.9964650000000006</v>
       </c>
-      <c r="D4" s="37">
+      <c r="H4" s="37">
         <v>3.77</v>
       </c>
-      <c r="E4" s="36" t="s">
-        <v>61</v>
-      </c>
-      <c r="F4" s="39">
-        <v>242</v>
-      </c>
-      <c r="G4" s="39" t="s">
-        <v>41</v>
-      </c>
-      <c r="H4" s="36" t="s">
+      <c r="I4" s="36" t="s">
         <v>65</v>
       </c>
-      <c r="I4" s="36" t="s">
+      <c r="J4" s="36" t="s">
         <v>180</v>
       </c>
-      <c r="J4" s="36" t="s">
+      <c r="K4" s="36" t="s">
         <v>220</v>
-      </c>
-      <c r="K4" s="36" t="s">
-        <v>189</v>
       </c>
       <c r="L4" s="2"/>
       <c r="M4" s="2" t="s">
@@ -7550,35 +7553,35 @@
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A5" s="31"/>
-      <c r="B5" s="36" t="s">
+      <c r="B5" s="4" t="s">
         <v>64</v>
       </c>
-      <c r="C5" s="37">
+      <c r="C5" s="36" t="s">
+        <v>63</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>216</v>
+      </c>
+      <c r="E5" s="39">
+        <v>19</v>
+      </c>
+      <c r="F5" s="39">
+        <v>28312</v>
+      </c>
+      <c r="G5" s="37">
         <v>9.9964650000000006</v>
       </c>
-      <c r="D5" s="37">
+      <c r="H5" s="37">
         <v>3.7791410000000001</v>
       </c>
-      <c r="E5" s="36" t="s">
-        <v>63</v>
-      </c>
-      <c r="F5" s="39">
-        <v>19</v>
-      </c>
-      <c r="G5" s="39">
-        <v>28312</v>
-      </c>
-      <c r="H5" s="36" t="s">
+      <c r="I5" s="36" t="s">
         <v>65</v>
       </c>
-      <c r="I5" s="36" t="s">
+      <c r="J5" s="36" t="s">
         <v>180</v>
       </c>
-      <c r="J5" s="36" t="s">
+      <c r="K5" s="36" t="s">
         <v>220</v>
-      </c>
-      <c r="K5" s="36" t="s">
-        <v>216</v>
       </c>
       <c r="L5" s="2"/>
       <c r="M5" s="2" t="s">
@@ -7589,35 +7592,35 @@
       <c r="A6" s="12" t="s">
         <v>131</v>
       </c>
-      <c r="B6" s="36" t="s">
+      <c r="B6" s="4" t="s">
         <v>71</v>
       </c>
-      <c r="C6" s="37">
+      <c r="C6" s="36" t="s">
+        <v>70</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>189</v>
+      </c>
+      <c r="E6" s="39" t="s">
+        <v>41</v>
+      </c>
+      <c r="F6" s="39">
+        <v>29066</v>
+      </c>
+      <c r="G6" s="37">
         <v>9.2689000000000004</v>
       </c>
-      <c r="D6" s="37">
+      <c r="H6" s="37">
         <v>4.45</v>
       </c>
-      <c r="E6" s="36" t="s">
-        <v>70</v>
-      </c>
-      <c r="F6" s="39" t="s">
-        <v>41</v>
-      </c>
-      <c r="G6" s="39">
-        <v>29066</v>
-      </c>
-      <c r="H6" s="36" t="s">
+      <c r="I6" s="36" t="s">
         <v>65</v>
       </c>
-      <c r="I6" s="36" t="s">
+      <c r="J6" s="36" t="s">
         <v>180</v>
       </c>
-      <c r="J6" s="36" t="s">
+      <c r="K6" s="36" t="s">
         <v>220</v>
-      </c>
-      <c r="K6" s="36" t="s">
-        <v>216</v>
       </c>
       <c r="L6" s="2"/>
       <c r="M6" s="2" t="s">
@@ -7628,35 +7631,35 @@
       <c r="A7" s="7" t="s">
         <v>110</v>
       </c>
-      <c r="B7" s="36" t="s">
+      <c r="B7" s="4" t="s">
         <v>111</v>
       </c>
-      <c r="C7" s="37">
+      <c r="C7" s="36" t="s">
+        <v>110</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>217</v>
+      </c>
+      <c r="E7" s="39">
+        <v>300</v>
+      </c>
+      <c r="F7" s="39" t="s">
+        <v>41</v>
+      </c>
+      <c r="G7" s="37">
         <v>9.4</v>
       </c>
-      <c r="D7" s="37">
+      <c r="H7" s="37">
         <v>4.67</v>
       </c>
-      <c r="E7" s="36" t="s">
-        <v>110</v>
-      </c>
-      <c r="F7" s="39">
-        <v>300</v>
-      </c>
-      <c r="G7" s="39" t="s">
-        <v>41</v>
-      </c>
-      <c r="H7" s="36" t="s">
+      <c r="I7" s="36" t="s">
         <v>65</v>
       </c>
-      <c r="I7" s="36" t="s">
+      <c r="J7" s="36" t="s">
         <v>180</v>
       </c>
-      <c r="J7" s="36" t="s">
+      <c r="K7" s="36" t="s">
         <v>220</v>
-      </c>
-      <c r="K7" s="36" t="s">
-        <v>217</v>
       </c>
       <c r="L7" s="2"/>
       <c r="M7" s="2" t="s">
@@ -7667,35 +7670,35 @@
       <c r="A8" s="7" t="s">
         <v>133</v>
       </c>
-      <c r="B8" s="36" t="s">
+      <c r="B8" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="C8" s="37">
+      <c r="C8" s="36" t="s">
+        <v>133</v>
+      </c>
+      <c r="D8" s="2" t="s">
+        <v>189</v>
+      </c>
+      <c r="E8" s="39">
+        <v>1191</v>
+      </c>
+      <c r="F8" s="39" t="s">
+        <v>41</v>
+      </c>
+      <c r="G8" s="37">
         <v>10.581908</v>
       </c>
-      <c r="D8" s="37">
+      <c r="H8" s="37">
         <v>5.5660420000000004</v>
       </c>
-      <c r="E8" s="36" t="s">
-        <v>133</v>
-      </c>
-      <c r="F8" s="39">
-        <v>1191</v>
-      </c>
-      <c r="G8" s="39" t="s">
-        <v>41</v>
-      </c>
-      <c r="H8" s="36" t="s">
+      <c r="I8" s="36" t="s">
         <v>65</v>
       </c>
-      <c r="I8" s="36" t="s">
+      <c r="J8" s="36" t="s">
         <v>183</v>
       </c>
-      <c r="J8" s="36" t="s">
+      <c r="K8" s="36" t="s">
         <v>220</v>
-      </c>
-      <c r="K8" s="36" t="s">
-        <v>189</v>
       </c>
       <c r="L8" s="2"/>
       <c r="M8" s="2" t="s">
@@ -7706,35 +7709,35 @@
       <c r="A9" s="7" t="s">
         <v>127</v>
       </c>
-      <c r="B9" s="36" t="s">
+      <c r="B9" s="4" t="s">
         <v>77</v>
       </c>
-      <c r="C9" s="37">
+      <c r="C9" s="36" t="s">
+        <v>76</v>
+      </c>
+      <c r="D9" s="2" t="s">
+        <v>189</v>
+      </c>
+      <c r="E9" s="39">
+        <v>2273</v>
+      </c>
+      <c r="F9" s="39">
+        <v>23662</v>
+      </c>
+      <c r="G9" s="37">
         <v>10.240641</v>
       </c>
-      <c r="D9" s="37">
+      <c r="H9" s="37">
         <v>5.9336890000000002</v>
       </c>
-      <c r="E9" s="36" t="s">
-        <v>76</v>
-      </c>
-      <c r="F9" s="39">
-        <v>2273</v>
-      </c>
-      <c r="G9" s="39">
-        <v>23662</v>
-      </c>
-      <c r="H9" s="36" t="s">
+      <c r="I9" s="36" t="s">
         <v>65</v>
       </c>
-      <c r="I9" s="36" t="s">
+      <c r="J9" s="36" t="s">
         <v>183</v>
       </c>
-      <c r="J9" s="36" t="s">
+      <c r="K9" s="36" t="s">
         <v>220</v>
-      </c>
-      <c r="K9" s="36" t="s">
-        <v>216</v>
       </c>
       <c r="L9" s="2"/>
       <c r="M9" s="2" t="s">
@@ -7745,35 +7748,35 @@
       <c r="A10" s="7" t="s">
         <v>78</v>
       </c>
-      <c r="B10" s="36" t="s">
+      <c r="B10" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="C10" s="37">
+      <c r="C10" s="36" t="s">
+        <v>78</v>
+      </c>
+      <c r="D10" s="2" t="s">
+        <v>189</v>
+      </c>
+      <c r="E10" s="39">
+        <v>2015</v>
+      </c>
+      <c r="F10" s="39" t="s">
+        <v>41</v>
+      </c>
+      <c r="G10" s="37">
         <v>10.348549</v>
       </c>
-      <c r="D10" s="37">
+      <c r="H10" s="37">
         <v>6.0892730000000004</v>
       </c>
-      <c r="E10" s="36" t="s">
-        <v>78</v>
-      </c>
-      <c r="F10" s="39">
-        <v>2015</v>
-      </c>
-      <c r="G10" s="39" t="s">
-        <v>41</v>
-      </c>
-      <c r="H10" s="36" t="s">
+      <c r="I10" s="36" t="s">
         <v>65</v>
       </c>
-      <c r="I10" s="36" t="s">
+      <c r="J10" s="36" t="s">
         <v>183</v>
       </c>
-      <c r="J10" s="36" t="s">
+      <c r="K10" s="36" t="s">
         <v>220</v>
-      </c>
-      <c r="K10" s="36" t="s">
-        <v>189</v>
       </c>
       <c r="L10" s="2"/>
       <c r="M10" s="2" t="s">
@@ -7784,35 +7787,35 @@
       <c r="A11" s="7" t="s">
         <v>134</v>
       </c>
-      <c r="B11" s="36" t="s">
+      <c r="B11" s="4" t="s">
         <v>79</v>
       </c>
-      <c r="C11" s="37">
+      <c r="C11" s="36" t="s">
+        <v>15</v>
+      </c>
+      <c r="D11" s="2" t="s">
+        <v>189</v>
+      </c>
+      <c r="E11" s="39">
+        <v>1160</v>
+      </c>
+      <c r="F11" s="39">
+        <v>27428</v>
+      </c>
+      <c r="G11" s="37">
         <v>13.58333</v>
       </c>
-      <c r="D11" s="37">
+      <c r="H11" s="37">
         <v>7.25</v>
       </c>
-      <c r="E11" s="36" t="s">
-        <v>15</v>
-      </c>
-      <c r="F11" s="39">
-        <v>1160</v>
-      </c>
-      <c r="G11" s="39">
-        <v>27428</v>
-      </c>
-      <c r="H11" s="36" t="s">
+      <c r="I11" s="36" t="s">
         <v>65</v>
       </c>
-      <c r="I11" s="36" t="s">
+      <c r="J11" s="36" t="s">
         <v>183</v>
       </c>
-      <c r="J11" s="36" t="s">
+      <c r="K11" s="36" t="s">
         <v>220</v>
-      </c>
-      <c r="K11" s="36" t="s">
-        <v>217</v>
       </c>
       <c r="L11" s="2">
         <v>6</v>
@@ -7825,35 +7828,35 @@
       <c r="A12" s="7" t="s">
         <v>135</v>
       </c>
-      <c r="B12" s="36" t="s">
+      <c r="B12" s="4" t="s">
         <v>80</v>
       </c>
-      <c r="C12" s="37">
+      <c r="C12" s="36" t="s">
+        <v>10</v>
+      </c>
+      <c r="D12" s="2" t="s">
+        <v>216</v>
+      </c>
+      <c r="E12" s="39">
+        <v>1110</v>
+      </c>
+      <c r="F12" s="39">
+        <v>27416</v>
+      </c>
+      <c r="G12" s="37">
         <v>13.733333333333301</v>
       </c>
-      <c r="D12" s="37">
+      <c r="H12" s="37">
         <v>7.31666666666667</v>
       </c>
-      <c r="E12" s="36" t="s">
-        <v>10</v>
-      </c>
-      <c r="F12" s="39">
-        <v>1110</v>
-      </c>
-      <c r="G12" s="39">
-        <v>27416</v>
-      </c>
-      <c r="H12" s="36" t="s">
+      <c r="I12" s="36" t="s">
         <v>65</v>
       </c>
-      <c r="I12" s="36" t="s">
+      <c r="J12" s="36" t="s">
         <v>183</v>
       </c>
-      <c r="J12" s="36" t="s">
+      <c r="K12" s="36" t="s">
         <v>220</v>
-      </c>
-      <c r="K12" s="36" t="s">
-        <v>216</v>
       </c>
       <c r="L12" s="2"/>
       <c r="M12" s="2" t="s">
@@ -7864,35 +7867,35 @@
       <c r="A13" s="12" t="s">
         <v>122</v>
       </c>
-      <c r="B13" s="36" t="s">
+      <c r="B13" s="4" t="s">
         <v>92</v>
       </c>
-      <c r="C13" s="37">
+      <c r="C13" s="36" t="s">
+        <v>91</v>
+      </c>
+      <c r="D13" s="2" t="s">
+        <v>217</v>
+      </c>
+      <c r="E13" s="39">
+        <v>350</v>
+      </c>
+      <c r="F13" s="39" t="s">
+        <v>41</v>
+      </c>
+      <c r="G13" s="37">
         <v>11.77</v>
       </c>
-      <c r="D13" s="37">
+      <c r="H13" s="37">
         <v>-0.72</v>
       </c>
-      <c r="E13" s="36" t="s">
-        <v>91</v>
-      </c>
-      <c r="F13" s="39">
-        <v>350</v>
-      </c>
-      <c r="G13" s="39" t="s">
-        <v>41</v>
-      </c>
-      <c r="H13" s="36" t="s">
+      <c r="I13" s="36" t="s">
         <v>169</v>
       </c>
-      <c r="I13" s="36" t="s">
+      <c r="J13" s="36" t="s">
         <v>180</v>
       </c>
-      <c r="J13" s="36" t="s">
+      <c r="K13" s="36" t="s">
         <v>222</v>
-      </c>
-      <c r="K13" s="36" t="s">
-        <v>217</v>
       </c>
       <c r="L13" s="2"/>
       <c r="M13" s="2" t="s">
@@ -7903,35 +7906,35 @@
       <c r="A14" s="12" t="s">
         <v>123</v>
       </c>
-      <c r="B14" s="36" t="s">
+      <c r="B14" s="4" t="s">
         <v>94</v>
       </c>
-      <c r="C14" s="37">
+      <c r="C14" s="36" t="s">
+        <v>93</v>
+      </c>
+      <c r="D14" s="2" t="s">
+        <v>217</v>
+      </c>
+      <c r="E14" s="39">
+        <v>20</v>
+      </c>
+      <c r="F14" s="39" t="s">
+        <v>41</v>
+      </c>
+      <c r="G14" s="37">
         <v>10.47</v>
       </c>
-      <c r="D14" s="37">
+      <c r="H14" s="37">
         <v>-0.2</v>
       </c>
-      <c r="E14" s="36" t="s">
-        <v>93</v>
-      </c>
-      <c r="F14" s="39">
-        <v>20</v>
-      </c>
-      <c r="G14" s="39" t="s">
-        <v>41</v>
-      </c>
-      <c r="H14" s="36" t="s">
+      <c r="I14" s="36" t="s">
         <v>169</v>
       </c>
-      <c r="I14" s="36" t="s">
+      <c r="J14" s="36" t="s">
         <v>180</v>
       </c>
-      <c r="J14" s="36" t="s">
+      <c r="K14" s="36" t="s">
         <v>220</v>
-      </c>
-      <c r="K14" s="36" t="s">
-        <v>217</v>
       </c>
       <c r="L14" s="2"/>
       <c r="M14" s="2" t="s">
@@ -7942,35 +7945,35 @@
       <c r="A15" s="12" t="s">
         <v>95</v>
       </c>
-      <c r="B15" s="36" t="s">
+      <c r="B15" s="4" t="s">
         <v>96</v>
       </c>
-      <c r="C15" s="37">
+      <c r="C15" s="36" t="s">
+        <v>95</v>
+      </c>
+      <c r="D15" s="2" t="s">
+        <v>217</v>
+      </c>
+      <c r="E15" s="39">
+        <v>5</v>
+      </c>
+      <c r="F15" s="39" t="s">
+        <v>41</v>
+      </c>
+      <c r="G15" s="37">
         <v>9.35</v>
       </c>
-      <c r="D15" s="37">
+      <c r="H15" s="37">
         <v>-0.17</v>
       </c>
-      <c r="E15" s="36" t="s">
-        <v>95</v>
-      </c>
-      <c r="F15" s="39">
-        <v>5</v>
-      </c>
-      <c r="G15" s="39" t="s">
-        <v>41</v>
-      </c>
-      <c r="H15" s="36" t="s">
+      <c r="I15" s="36" t="s">
         <v>169</v>
       </c>
-      <c r="I15" s="36" t="s">
+      <c r="J15" s="36" t="s">
         <v>180</v>
       </c>
-      <c r="J15" s="36" t="s">
+      <c r="K15" s="36" t="s">
         <v>220</v>
-      </c>
-      <c r="K15" s="36" t="s">
-        <v>217</v>
       </c>
       <c r="L15" s="2"/>
       <c r="M15" s="2" t="s">
@@ -7981,35 +7984,35 @@
       <c r="A16" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="B16" s="33" t="s">
+      <c r="B16" s="42" t="s">
         <v>45</v>
       </c>
-      <c r="C16" s="34">
+      <c r="C16" s="33" t="s">
+        <v>8</v>
+      </c>
+      <c r="D16" s="9" t="s">
+        <v>216</v>
+      </c>
+      <c r="E16" s="35">
+        <v>103</v>
+      </c>
+      <c r="F16" s="35">
+        <v>27167</v>
+      </c>
+      <c r="G16" s="34">
         <v>11.86641</v>
       </c>
-      <c r="D16" s="34">
+      <c r="H16" s="34">
         <v>-4.7662000000000004</v>
       </c>
-      <c r="E16" s="33" t="s">
-        <v>8</v>
-      </c>
-      <c r="F16" s="35">
-        <v>103</v>
-      </c>
-      <c r="G16" s="35">
-        <v>27167</v>
-      </c>
-      <c r="H16" s="33" t="s">
+      <c r="I16" s="33" t="s">
         <v>44</v>
       </c>
-      <c r="I16" s="33" t="s">
+      <c r="J16" s="33" t="s">
         <v>180</v>
       </c>
-      <c r="J16" s="33" t="s">
+      <c r="K16" s="33" t="s">
         <v>219</v>
-      </c>
-      <c r="K16" s="33" t="s">
-        <v>216</v>
       </c>
       <c r="L16" s="9"/>
       <c r="M16" s="2" t="s">
@@ -8020,35 +8023,35 @@
       <c r="A17" s="30" t="s">
         <v>128</v>
       </c>
-      <c r="B17" s="36" t="s">
+      <c r="B17" s="4" t="s">
         <v>48</v>
       </c>
-      <c r="C17" s="37">
+      <c r="C17" s="36" t="s">
+        <v>47</v>
+      </c>
+      <c r="D17" s="9" t="s">
+        <v>216</v>
+      </c>
+      <c r="E17" s="38">
+        <v>75</v>
+      </c>
+      <c r="F17" s="39">
+        <v>27159</v>
+      </c>
+      <c r="G17" s="37">
         <v>11.85</v>
       </c>
-      <c r="D17" s="37">
+      <c r="H17" s="37">
         <v>-4.75</v>
       </c>
-      <c r="E17" s="36" t="s">
-        <v>47</v>
-      </c>
-      <c r="F17" s="38">
-        <v>75</v>
-      </c>
-      <c r="G17" s="39">
-        <v>27159</v>
-      </c>
-      <c r="H17" s="36" t="s">
+      <c r="I17" s="36" t="s">
         <v>44</v>
       </c>
-      <c r="I17" s="33" t="s">
+      <c r="J17" s="33" t="s">
         <v>180</v>
       </c>
-      <c r="J17" s="33" t="s">
+      <c r="K17" s="33" t="s">
         <v>219</v>
-      </c>
-      <c r="K17" s="33" t="s">
-        <v>216</v>
       </c>
       <c r="L17" s="2"/>
       <c r="M17" s="2" t="s">
@@ -8057,35 +8060,35 @@
     </row>
     <row r="18" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A18" s="31"/>
-      <c r="B18" s="36" t="s">
+      <c r="B18" s="4" t="s">
         <v>50</v>
       </c>
-      <c r="C18" s="37">
+      <c r="C18" s="36" t="s">
+        <v>49</v>
+      </c>
+      <c r="D18" s="9" t="s">
+        <v>216</v>
+      </c>
+      <c r="E18" s="38">
+        <v>76</v>
+      </c>
+      <c r="F18" s="39">
+        <v>27159</v>
+      </c>
+      <c r="G18" s="37">
         <v>11.850277999999999</v>
       </c>
-      <c r="D18" s="37">
+      <c r="H18" s="37">
         <v>-4.7420099999999996</v>
       </c>
-      <c r="E18" s="36" t="s">
-        <v>49</v>
-      </c>
-      <c r="F18" s="38">
-        <v>76</v>
-      </c>
-      <c r="G18" s="39">
-        <v>27159</v>
-      </c>
-      <c r="H18" s="36" t="s">
+      <c r="I18" s="36" t="s">
         <v>44</v>
       </c>
-      <c r="I18" s="33" t="s">
+      <c r="J18" s="33" t="s">
         <v>180</v>
       </c>
-      <c r="J18" s="33" t="s">
+      <c r="K18" s="33" t="s">
         <v>219</v>
-      </c>
-      <c r="K18" s="33" t="s">
-        <v>216</v>
       </c>
       <c r="L18" s="2"/>
       <c r="M18" s="2" t="s">
@@ -8096,35 +8099,35 @@
       <c r="A19" s="12" t="s">
         <v>13</v>
       </c>
-      <c r="B19" s="36" t="s">
+      <c r="B19" s="4" t="s">
         <v>52</v>
       </c>
-      <c r="C19" s="37">
+      <c r="C19" s="36" t="s">
+        <v>13</v>
+      </c>
+      <c r="D19" s="9" t="s">
+        <v>216</v>
+      </c>
+      <c r="E19" s="39">
+        <v>13</v>
+      </c>
+      <c r="F19" s="39">
+        <v>28406</v>
+      </c>
+      <c r="G19" s="37">
         <v>12</v>
       </c>
-      <c r="D19" s="37">
+      <c r="H19" s="37">
         <v>-4.2699999999999996</v>
       </c>
-      <c r="E19" s="36" t="s">
-        <v>13</v>
-      </c>
-      <c r="F19" s="39">
-        <v>13</v>
-      </c>
-      <c r="G19" s="39">
-        <v>28406</v>
-      </c>
-      <c r="H19" s="36" t="s">
+      <c r="I19" s="36" t="s">
         <v>44</v>
       </c>
-      <c r="I19" s="33" t="s">
+      <c r="J19" s="33" t="s">
         <v>180</v>
       </c>
-      <c r="J19" s="33" t="s">
+      <c r="K19" s="33" t="s">
         <v>220</v>
-      </c>
-      <c r="K19" s="33" t="s">
-        <v>216</v>
       </c>
       <c r="L19" s="2">
         <v>8</v>
@@ -8137,35 +8140,35 @@
       <c r="A20" s="30" t="s">
         <v>4</v>
       </c>
-      <c r="B20" s="36" t="s">
+      <c r="B20" s="4" t="s">
         <v>55</v>
       </c>
-      <c r="C20" s="37">
+      <c r="C20" s="36" t="s">
+        <v>4</v>
+      </c>
+      <c r="D20" s="2" t="s">
+        <v>216</v>
+      </c>
+      <c r="E20" s="39">
+        <v>21</v>
+      </c>
+      <c r="F20" s="39">
+        <v>28227</v>
+      </c>
+      <c r="G20" s="37">
         <v>12.8</v>
       </c>
-      <c r="D20" s="37">
+      <c r="H20" s="37">
         <v>-3.8361109999999998</v>
       </c>
-      <c r="E20" s="36" t="s">
-        <v>4</v>
-      </c>
-      <c r="F20" s="39">
-        <v>21</v>
-      </c>
-      <c r="G20" s="39">
-        <v>28227</v>
-      </c>
-      <c r="H20" s="36" t="s">
+      <c r="I20" s="36" t="s">
         <v>44</v>
       </c>
-      <c r="I20" s="36" t="s">
+      <c r="J20" s="36" t="s">
         <v>180</v>
       </c>
-      <c r="J20" s="36" t="s">
+      <c r="K20" s="36" t="s">
         <v>220</v>
-      </c>
-      <c r="K20" s="36" t="s">
-        <v>216</v>
       </c>
       <c r="L20" s="2"/>
       <c r="M20" s="2" t="s">
@@ -8174,35 +8177,35 @@
     </row>
     <row r="21" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A21" s="31"/>
-      <c r="B21" s="36" t="s">
+      <c r="B21" s="4" t="s">
         <v>56</v>
       </c>
-      <c r="C21" s="37">
+      <c r="C21" s="36" t="s">
+        <v>4</v>
+      </c>
+      <c r="D21" s="2" t="s">
+        <v>216</v>
+      </c>
+      <c r="E21" s="39">
+        <v>22</v>
+      </c>
+      <c r="F21" s="39">
+        <v>28227</v>
+      </c>
+      <c r="G21" s="37">
         <v>12.804167</v>
       </c>
-      <c r="D21" s="37">
+      <c r="H21" s="37">
         <v>-3.835556</v>
       </c>
-      <c r="E21" s="36" t="s">
-        <v>4</v>
-      </c>
-      <c r="F21" s="39">
-        <v>22</v>
-      </c>
-      <c r="G21" s="39">
-        <v>28227</v>
-      </c>
-      <c r="H21" s="36" t="s">
+      <c r="I21" s="36" t="s">
         <v>44</v>
       </c>
-      <c r="I21" s="36" t="s">
+      <c r="J21" s="36" t="s">
         <v>180</v>
       </c>
-      <c r="J21" s="36" t="s">
+      <c r="K21" s="36" t="s">
         <v>220</v>
-      </c>
-      <c r="K21" s="36" t="s">
-        <v>216</v>
       </c>
       <c r="L21" s="2"/>
       <c r="M21" s="2" t="s">
@@ -8213,35 +8216,35 @@
       <c r="A22" s="30" t="s">
         <v>129</v>
       </c>
-      <c r="B22" s="36" t="s">
+      <c r="B22" s="4" t="s">
         <v>54</v>
       </c>
-      <c r="C22" s="37">
+      <c r="C22" s="36" t="s">
+        <v>7</v>
+      </c>
+      <c r="D22" s="9" t="s">
+        <v>216</v>
+      </c>
+      <c r="E22" s="39">
+        <v>10</v>
+      </c>
+      <c r="F22" s="39">
+        <v>28301</v>
+      </c>
+      <c r="G22" s="37">
         <v>15.383330000000001</v>
       </c>
-      <c r="D22" s="37">
+      <c r="H22" s="37">
         <v>-4.0750000000000002</v>
       </c>
-      <c r="E22" s="36" t="s">
-        <v>7</v>
-      </c>
-      <c r="F22" s="39">
-        <v>10</v>
-      </c>
-      <c r="G22" s="39">
-        <v>28301</v>
-      </c>
-      <c r="H22" s="36" t="s">
+      <c r="I22" s="36" t="s">
         <v>44</v>
       </c>
-      <c r="I22" s="36" t="s">
+      <c r="J22" s="36" t="s">
         <v>181</v>
       </c>
-      <c r="J22" s="36" t="s">
+      <c r="K22" s="36" t="s">
         <v>220</v>
-      </c>
-      <c r="K22" s="33" t="s">
-        <v>216</v>
       </c>
       <c r="L22" s="2"/>
       <c r="M22" s="2" t="s">
@@ -8250,35 +8253,35 @@
     </row>
     <row r="23" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A23" s="31"/>
-      <c r="B23" s="36" t="s">
+      <c r="B23" s="4" t="s">
         <v>53</v>
       </c>
-      <c r="C23" s="37">
+      <c r="C23" s="36" t="s">
+        <v>7</v>
+      </c>
+      <c r="D23" s="9" t="s">
+        <v>216</v>
+      </c>
+      <c r="E23" s="39">
+        <v>9</v>
+      </c>
+      <c r="F23" s="39">
+        <v>28301</v>
+      </c>
+      <c r="G23" s="37">
         <v>15.383333</v>
       </c>
-      <c r="D23" s="37">
+      <c r="H23" s="37">
         <v>-4.0750000000000002</v>
       </c>
-      <c r="E23" s="36" t="s">
-        <v>7</v>
-      </c>
-      <c r="F23" s="39">
-        <v>9</v>
-      </c>
-      <c r="G23" s="39">
-        <v>28301</v>
-      </c>
-      <c r="H23" s="36" t="s">
+      <c r="I23" s="36" t="s">
         <v>44</v>
       </c>
-      <c r="I23" s="36" t="s">
+      <c r="J23" s="36" t="s">
         <v>181</v>
       </c>
-      <c r="J23" s="36" t="s">
+      <c r="K23" s="36" t="s">
         <v>220</v>
-      </c>
-      <c r="K23" s="33" t="s">
-        <v>216</v>
       </c>
       <c r="L23" s="2"/>
       <c r="M23" s="2" t="s">
@@ -8289,35 +8292,35 @@
       <c r="A24" s="30" t="s">
         <v>3</v>
       </c>
-      <c r="B24" s="36" t="s">
+      <c r="B24" s="4" t="s">
         <v>58</v>
       </c>
-      <c r="C24" s="37">
+      <c r="C24" s="36" t="s">
+        <v>57</v>
+      </c>
+      <c r="D24" s="2" t="s">
+        <v>216</v>
+      </c>
+      <c r="E24" s="39">
+        <v>15</v>
+      </c>
+      <c r="F24" s="39">
+        <v>27149</v>
+      </c>
+      <c r="G24" s="37">
         <v>15.350277999999999</v>
       </c>
-      <c r="D24" s="37">
+      <c r="H24" s="37">
         <v>-3.516667</v>
       </c>
-      <c r="E24" s="36" t="s">
-        <v>57</v>
-      </c>
-      <c r="F24" s="39">
-        <v>15</v>
-      </c>
-      <c r="G24" s="39">
-        <v>27149</v>
-      </c>
-      <c r="H24" s="36" t="s">
+      <c r="I24" s="36" t="s">
         <v>44</v>
       </c>
-      <c r="I24" s="36" t="s">
+      <c r="J24" s="36" t="s">
         <v>181</v>
       </c>
-      <c r="J24" s="36" t="s">
+      <c r="K24" s="36" t="s">
         <v>222</v>
-      </c>
-      <c r="K24" s="36" t="s">
-        <v>216</v>
       </c>
       <c r="L24" s="2"/>
       <c r="M24" s="2" t="s">
@@ -8326,35 +8329,35 @@
     </row>
     <row r="25" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A25" s="31"/>
-      <c r="B25" s="36" t="s">
+      <c r="B25" s="4" t="s">
         <v>60</v>
       </c>
-      <c r="C25" s="37">
+      <c r="C25" s="36" t="s">
+        <v>59</v>
+      </c>
+      <c r="D25" s="2" t="s">
+        <v>216</v>
+      </c>
+      <c r="E25" s="39">
+        <v>16</v>
+      </c>
+      <c r="F25" s="39">
+        <v>27149</v>
+      </c>
+      <c r="G25" s="37">
         <v>15.35116</v>
       </c>
-      <c r="D25" s="37">
+      <c r="H25" s="37">
         <v>-3.5138500000000001</v>
       </c>
-      <c r="E25" s="36" t="s">
-        <v>59</v>
-      </c>
-      <c r="F25" s="39">
-        <v>16</v>
-      </c>
-      <c r="G25" s="39">
-        <v>27149</v>
-      </c>
-      <c r="H25" s="36" t="s">
+      <c r="I25" s="36" t="s">
         <v>44</v>
       </c>
-      <c r="I25" s="36" t="s">
+      <c r="J25" s="36" t="s">
         <v>181</v>
       </c>
-      <c r="J25" s="36" t="s">
+      <c r="K25" s="36" t="s">
         <v>222</v>
-      </c>
-      <c r="K25" s="36" t="s">
-        <v>216</v>
       </c>
       <c r="L25" s="2"/>
       <c r="M25" s="2" t="s">
@@ -8365,35 +8368,35 @@
       <c r="A26" s="30" t="s">
         <v>97</v>
       </c>
-      <c r="B26" s="36" t="s">
+      <c r="B26" s="4" t="s">
         <v>116</v>
       </c>
-      <c r="C26" s="37">
+      <c r="C26" s="36" t="s">
+        <v>97</v>
+      </c>
+      <c r="D26" s="2" t="s">
+        <v>217</v>
+      </c>
+      <c r="E26" s="39">
+        <v>327</v>
+      </c>
+      <c r="F26" s="39" t="s">
+        <v>41</v>
+      </c>
+      <c r="G26" s="37">
         <v>17.75</v>
       </c>
-      <c r="D26" s="37">
+      <c r="H26" s="37">
         <v>1.175</v>
       </c>
-      <c r="E26" s="36" t="s">
-        <v>97</v>
-      </c>
-      <c r="F26" s="39">
-        <v>327</v>
-      </c>
-      <c r="G26" s="39" t="s">
-        <v>41</v>
-      </c>
-      <c r="H26" s="36" t="s">
+      <c r="I26" s="36" t="s">
         <v>44</v>
       </c>
-      <c r="I26" s="36" t="s">
+      <c r="J26" s="36" t="s">
         <v>227</v>
       </c>
-      <c r="J26" s="36" t="s">
+      <c r="K26" s="36" t="s">
         <v>223</v>
-      </c>
-      <c r="K26" s="36" t="s">
-        <v>217</v>
       </c>
       <c r="L26" s="2"/>
       <c r="M26" s="2" t="s">
@@ -8402,35 +8405,35 @@
     </row>
     <row r="27" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A27" s="32"/>
-      <c r="B27" s="36" t="s">
+      <c r="B27" s="4" t="s">
         <v>115</v>
       </c>
-      <c r="C27" s="37">
+      <c r="C27" s="36" t="s">
+        <v>97</v>
+      </c>
+      <c r="D27" s="2" t="s">
+        <v>217</v>
+      </c>
+      <c r="E27" s="39">
+        <v>327</v>
+      </c>
+      <c r="F27" s="39" t="s">
+        <v>41</v>
+      </c>
+      <c r="G27" s="37">
         <v>17.8</v>
       </c>
-      <c r="D27" s="37">
+      <c r="H27" s="37">
         <v>1.18</v>
       </c>
-      <c r="E27" s="36" t="s">
-        <v>97</v>
-      </c>
-      <c r="F27" s="39">
-        <v>327</v>
-      </c>
-      <c r="G27" s="39" t="s">
-        <v>41</v>
-      </c>
-      <c r="H27" s="36" t="s">
+      <c r="I27" s="36" t="s">
         <v>44</v>
       </c>
-      <c r="I27" s="36" t="s">
+      <c r="J27" s="36" t="s">
         <v>227</v>
       </c>
-      <c r="J27" s="36" t="s">
+      <c r="K27" s="36" t="s">
         <v>223</v>
-      </c>
-      <c r="K27" s="36" t="s">
-        <v>217</v>
       </c>
       <c r="L27" s="2"/>
       <c r="M27" s="2" t="s">
@@ -8439,35 +8442,35 @@
     </row>
     <row r="28" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A28" s="32"/>
-      <c r="B28" s="36" t="s">
+      <c r="B28" s="4" t="s">
         <v>88</v>
       </c>
-      <c r="C28" s="37">
+      <c r="C28" s="36" t="s">
+        <v>97</v>
+      </c>
+      <c r="D28" s="2" t="s">
+        <v>217</v>
+      </c>
+      <c r="E28" s="39">
+        <v>327</v>
+      </c>
+      <c r="F28" s="39" t="s">
+        <v>41</v>
+      </c>
+      <c r="G28" s="37">
         <v>17.639900000000001</v>
       </c>
-      <c r="D28" s="37">
+      <c r="H28" s="37">
         <v>1.1835</v>
       </c>
-      <c r="E28" s="36" t="s">
-        <v>97</v>
-      </c>
-      <c r="F28" s="39">
-        <v>327</v>
-      </c>
-      <c r="G28" s="39" t="s">
-        <v>41</v>
-      </c>
-      <c r="H28" s="36" t="s">
+      <c r="I28" s="36" t="s">
         <v>44</v>
       </c>
-      <c r="I28" s="36" t="s">
+      <c r="J28" s="36" t="s">
         <v>227</v>
       </c>
-      <c r="J28" s="36" t="s">
+      <c r="K28" s="36" t="s">
         <v>223</v>
-      </c>
-      <c r="K28" s="36" t="s">
-        <v>217</v>
       </c>
       <c r="L28" s="2"/>
       <c r="M28" s="2" t="s">
@@ -8476,35 +8479,35 @@
     </row>
     <row r="29" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A29" s="32"/>
-      <c r="B29" s="36" t="s">
+      <c r="B29" s="4" t="s">
         <v>117</v>
       </c>
-      <c r="C29" s="37">
+      <c r="C29" s="36" t="s">
+        <v>97</v>
+      </c>
+      <c r="D29" s="2" t="s">
+        <v>217</v>
+      </c>
+      <c r="E29" s="39">
+        <v>327</v>
+      </c>
+      <c r="F29" s="39" t="s">
+        <v>41</v>
+      </c>
+      <c r="G29" s="37">
         <v>17.7</v>
       </c>
-      <c r="D29" s="37">
+      <c r="H29" s="37">
         <v>1.1835</v>
       </c>
-      <c r="E29" s="36" t="s">
-        <v>97</v>
-      </c>
-      <c r="F29" s="39">
-        <v>327</v>
-      </c>
-      <c r="G29" s="39" t="s">
-        <v>41</v>
-      </c>
-      <c r="H29" s="36" t="s">
+      <c r="I29" s="36" t="s">
         <v>44</v>
       </c>
-      <c r="I29" s="36" t="s">
+      <c r="J29" s="36" t="s">
         <v>227</v>
       </c>
-      <c r="J29" s="36" t="s">
+      <c r="K29" s="36" t="s">
         <v>223</v>
-      </c>
-      <c r="K29" s="36" t="s">
-        <v>217</v>
       </c>
       <c r="L29" s="2"/>
       <c r="M29" s="2" t="s">
@@ -8513,35 +8516,35 @@
     </row>
     <row r="30" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A30" s="31"/>
-      <c r="B30" s="36" t="s">
+      <c r="B30" s="4" t="s">
         <v>118</v>
       </c>
-      <c r="C30" s="37">
+      <c r="C30" s="36" t="s">
+        <v>119</v>
+      </c>
+      <c r="D30" s="2" t="s">
+        <v>217</v>
+      </c>
+      <c r="E30" s="39">
+        <v>327</v>
+      </c>
+      <c r="F30" s="39" t="s">
+        <v>41</v>
+      </c>
+      <c r="G30" s="37">
         <v>17.48</v>
       </c>
-      <c r="D30" s="37">
+      <c r="H30" s="37">
         <v>1.2</v>
       </c>
-      <c r="E30" s="36" t="s">
-        <v>119</v>
-      </c>
-      <c r="F30" s="39">
-        <v>327</v>
-      </c>
-      <c r="G30" s="39" t="s">
-        <v>41</v>
-      </c>
-      <c r="H30" s="36" t="s">
+      <c r="I30" s="36" t="s">
         <v>44</v>
       </c>
-      <c r="I30" s="36" t="s">
+      <c r="J30" s="36" t="s">
         <v>227</v>
       </c>
-      <c r="J30" s="36" t="s">
+      <c r="K30" s="36" t="s">
         <v>223</v>
-      </c>
-      <c r="K30" s="36" t="s">
-        <v>217</v>
       </c>
       <c r="L30" s="2"/>
       <c r="M30" s="2" t="s">
@@ -8552,35 +8555,35 @@
       <c r="A31" s="7" t="s">
         <v>124</v>
       </c>
-      <c r="B31" s="36" t="s">
+      <c r="B31" s="21" t="s">
         <v>101</v>
       </c>
-      <c r="C31" s="37">
+      <c r="C31" s="36" t="s">
+        <v>100</v>
+      </c>
+      <c r="D31" s="2" t="s">
+        <v>113</v>
+      </c>
+      <c r="E31" s="39">
+        <v>370</v>
+      </c>
+      <c r="F31" s="39" t="s">
+        <v>41</v>
+      </c>
+      <c r="G31" s="37">
         <v>16.510000000000002</v>
       </c>
-      <c r="D31" s="37">
+      <c r="H31" s="37">
         <v>2.16</v>
       </c>
-      <c r="E31" s="36" t="s">
-        <v>100</v>
-      </c>
-      <c r="F31" s="39">
-        <v>370</v>
-      </c>
-      <c r="G31" s="39" t="s">
-        <v>41</v>
-      </c>
-      <c r="H31" s="36" t="s">
+      <c r="I31" s="36" t="s">
         <v>44</v>
       </c>
-      <c r="I31" s="36" t="s">
+      <c r="J31" s="36" t="s">
         <v>227</v>
       </c>
-      <c r="J31" s="36" t="s">
+      <c r="K31" s="36" t="s">
         <v>222</v>
-      </c>
-      <c r="K31" s="36" t="s">
-        <v>113</v>
       </c>
       <c r="L31" s="2"/>
       <c r="M31" s="2" t="s">
@@ -8591,35 +8594,35 @@
       <c r="A32" s="7" t="s">
         <v>148</v>
       </c>
-      <c r="B32" s="36" t="s">
+      <c r="B32" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="C32" s="37">
+      <c r="C32" s="36" t="s">
+        <v>147</v>
+      </c>
+      <c r="D32" s="2" t="s">
+        <v>189</v>
+      </c>
+      <c r="E32" s="39">
+        <v>396</v>
+      </c>
+      <c r="F32" s="39" t="s">
+        <v>41</v>
+      </c>
+      <c r="G32" s="37">
         <v>16.525130000000001</v>
       </c>
-      <c r="D32" s="37">
+      <c r="H32" s="37">
         <v>2.1872600000000002</v>
       </c>
-      <c r="E32" s="36" t="s">
-        <v>147</v>
-      </c>
-      <c r="F32" s="39">
-        <v>396</v>
-      </c>
-      <c r="G32" s="39" t="s">
-        <v>41</v>
-      </c>
-      <c r="H32" s="36" t="s">
+      <c r="I32" s="36" t="s">
         <v>44</v>
       </c>
-      <c r="I32" s="36" t="s">
+      <c r="J32" s="36" t="s">
         <v>227</v>
       </c>
-      <c r="J32" s="36" t="s">
+      <c r="K32" s="36" t="s">
         <v>222</v>
-      </c>
-      <c r="K32" s="36" t="s">
-        <v>189</v>
       </c>
       <c r="L32" s="2">
         <v>3</v>
@@ -8632,35 +8635,35 @@
       <c r="A33" s="12" t="s">
         <v>102</v>
       </c>
-      <c r="B33" s="36" t="s">
+      <c r="B33" s="4" t="s">
         <v>103</v>
       </c>
-      <c r="C33" s="37" t="s">
+      <c r="C33" s="36" t="s">
+        <v>102</v>
+      </c>
+      <c r="D33" s="2" t="s">
+        <v>217</v>
+      </c>
+      <c r="E33" s="39">
+        <v>390</v>
+      </c>
+      <c r="F33" s="39" t="s">
+        <v>41</v>
+      </c>
+      <c r="G33" s="37" t="s">
         <v>104</v>
       </c>
-      <c r="D33" s="37">
+      <c r="H33" s="37">
         <v>2.2405599999999999</v>
       </c>
-      <c r="E33" s="36" t="s">
-        <v>102</v>
-      </c>
-      <c r="F33" s="39">
-        <v>390</v>
-      </c>
-      <c r="G33" s="39" t="s">
-        <v>41</v>
-      </c>
-      <c r="H33" s="36" t="s">
+      <c r="I33" s="36" t="s">
         <v>44</v>
       </c>
-      <c r="I33" s="36" t="s">
+      <c r="J33" s="36" t="s">
         <v>227</v>
       </c>
-      <c r="J33" s="36" t="s">
+      <c r="K33" s="36" t="s">
         <v>222</v>
-      </c>
-      <c r="K33" s="36" t="s">
-        <v>217</v>
       </c>
       <c r="L33" s="2"/>
       <c r="M33" s="2" t="s">
@@ -8671,35 +8674,35 @@
       <c r="A34" s="30" t="s">
         <v>126</v>
       </c>
-      <c r="B34" s="36" t="s">
+      <c r="B34" s="4" t="s">
         <v>109</v>
       </c>
-      <c r="C34" s="37" t="s">
+      <c r="C34" s="36" t="s">
+        <v>108</v>
+      </c>
+      <c r="D34" s="2" t="s">
+        <v>217</v>
+      </c>
+      <c r="E34" s="39">
+        <v>573</v>
+      </c>
+      <c r="F34" s="39" t="s">
+        <v>41</v>
+      </c>
+      <c r="G34" s="37" t="s">
         <v>107</v>
       </c>
-      <c r="D34" s="37">
+      <c r="H34" s="37">
         <v>3.6635</v>
       </c>
-      <c r="E34" s="36" t="s">
-        <v>108</v>
-      </c>
-      <c r="F34" s="39">
-        <v>573</v>
-      </c>
-      <c r="G34" s="39" t="s">
-        <v>41</v>
-      </c>
-      <c r="H34" s="36" t="s">
+      <c r="I34" s="36" t="s">
         <v>72</v>
       </c>
-      <c r="I34" s="36" t="s">
+      <c r="J34" s="36" t="s">
         <v>227</v>
       </c>
-      <c r="J34" s="36" t="s">
+      <c r="K34" s="36" t="s">
         <v>223</v>
-      </c>
-      <c r="K34" s="36" t="s">
-        <v>217</v>
       </c>
       <c r="L34" s="2"/>
       <c r="M34" s="2" t="s">
@@ -8708,35 +8711,35 @@
     </row>
     <row r="35" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A35" s="32"/>
-      <c r="B35" s="36" t="s">
+      <c r="B35" s="4" t="s">
         <v>69</v>
       </c>
-      <c r="C35" s="37">
+      <c r="C35" s="36" t="s">
+        <v>68</v>
+      </c>
+      <c r="D35" s="2" t="s">
+        <v>189</v>
+      </c>
+      <c r="E35" s="39">
+        <v>448</v>
+      </c>
+      <c r="F35" s="39" t="s">
+        <v>41</v>
+      </c>
+      <c r="G35" s="37">
         <v>17.466696413370901</v>
       </c>
-      <c r="D35" s="37">
+      <c r="H35" s="37">
         <v>3.8333759074349998</v>
       </c>
-      <c r="E35" s="36" t="s">
-        <v>68</v>
-      </c>
-      <c r="F35" s="39">
-        <v>448</v>
-      </c>
-      <c r="G35" s="39" t="s">
-        <v>41</v>
-      </c>
-      <c r="H35" s="36" t="s">
+      <c r="I35" s="36" t="s">
         <v>72</v>
       </c>
-      <c r="I35" s="36" t="s">
+      <c r="J35" s="36" t="s">
         <v>227</v>
       </c>
-      <c r="J35" s="36" t="s">
+      <c r="K35" s="36" t="s">
         <v>223</v>
-      </c>
-      <c r="K35" s="36" t="s">
-        <v>189</v>
       </c>
       <c r="L35" s="2"/>
       <c r="M35" s="2" t="s">
@@ -8745,35 +8748,35 @@
     </row>
     <row r="36" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A36" s="31"/>
-      <c r="B36" s="36" t="s">
+      <c r="B36" s="4" t="s">
         <v>67</v>
       </c>
-      <c r="C36" s="37">
+      <c r="C36" s="36" t="s">
+        <v>66</v>
+      </c>
+      <c r="D36" s="2" t="s">
+        <v>189</v>
+      </c>
+      <c r="E36" s="39">
+        <v>459</v>
+      </c>
+      <c r="F36" s="39" t="s">
+        <v>41</v>
+      </c>
+      <c r="G36" s="37">
         <v>16.952105693051401</v>
       </c>
-      <c r="D36" s="37">
+      <c r="H36" s="37">
         <v>3.9759219365907299</v>
       </c>
-      <c r="E36" s="36" t="s">
-        <v>66</v>
-      </c>
-      <c r="F36" s="39">
-        <v>459</v>
-      </c>
-      <c r="G36" s="39" t="s">
-        <v>41</v>
-      </c>
-      <c r="H36" s="36" t="s">
+      <c r="I36" s="36" t="s">
         <v>72</v>
       </c>
-      <c r="I36" s="36" t="s">
+      <c r="J36" s="36" t="s">
         <v>227</v>
       </c>
-      <c r="J36" s="36" t="s">
+      <c r="K36" s="36" t="s">
         <v>223</v>
-      </c>
-      <c r="K36" s="36" t="s">
-        <v>189</v>
       </c>
       <c r="L36" s="2"/>
       <c r="M36" s="2" t="s">
@@ -8784,35 +8787,35 @@
       <c r="A37" s="30" t="s">
         <v>121</v>
       </c>
-      <c r="B37" s="36" t="s">
+      <c r="B37" s="4" t="s">
         <v>89</v>
       </c>
-      <c r="C37" s="37">
+      <c r="C37" s="36" t="s">
+        <v>98</v>
+      </c>
+      <c r="D37" s="2" t="s">
+        <v>217</v>
+      </c>
+      <c r="E37" s="39" t="s">
+        <v>41</v>
+      </c>
+      <c r="F37" s="39" t="s">
+        <v>41</v>
+      </c>
+      <c r="G37" s="37">
         <v>18.281984000000001</v>
       </c>
-      <c r="D37" s="37">
+      <c r="H37" s="37">
         <v>-1.9727680000000001</v>
       </c>
-      <c r="E37" s="36" t="s">
-        <v>98</v>
-      </c>
-      <c r="F37" s="39" t="s">
-        <v>41</v>
-      </c>
-      <c r="G37" s="39" t="s">
-        <v>41</v>
-      </c>
-      <c r="H37" s="36" t="s">
+      <c r="I37" s="36" t="s">
         <v>168</v>
       </c>
-      <c r="I37" s="36" t="s">
+      <c r="J37" s="36" t="s">
         <v>227</v>
       </c>
-      <c r="J37" s="36" t="s">
+      <c r="K37" s="36" t="s">
         <v>224</v>
-      </c>
-      <c r="K37" s="36" t="s">
-        <v>217</v>
       </c>
       <c r="L37" s="2"/>
       <c r="M37" s="2" t="s">
@@ -8821,35 +8824,35 @@
     </row>
     <row r="38" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A38" s="31"/>
-      <c r="B38" s="36" t="s">
+      <c r="B38" s="4" t="s">
         <v>90</v>
       </c>
-      <c r="C38" s="37">
+      <c r="C38" s="36" t="s">
+        <v>99</v>
+      </c>
+      <c r="D38" s="2" t="s">
+        <v>217</v>
+      </c>
+      <c r="E38" s="39" t="s">
+        <v>41</v>
+      </c>
+      <c r="F38" s="39" t="s">
+        <v>41</v>
+      </c>
+      <c r="G38" s="37">
         <v>18.320171999999999</v>
       </c>
-      <c r="D38" s="37">
+      <c r="H38" s="37">
         <v>-1.7745249999999999</v>
       </c>
-      <c r="E38" s="36" t="s">
-        <v>99</v>
-      </c>
-      <c r="F38" s="39" t="s">
-        <v>41</v>
-      </c>
-      <c r="G38" s="39" t="s">
-        <v>41</v>
-      </c>
-      <c r="H38" s="36" t="s">
+      <c r="I38" s="36" t="s">
         <v>168</v>
       </c>
-      <c r="I38" s="36" t="s">
+      <c r="J38" s="36" t="s">
         <v>227</v>
       </c>
-      <c r="J38" s="36" t="s">
+      <c r="K38" s="36" t="s">
         <v>224</v>
-      </c>
-      <c r="K38" s="36" t="s">
-        <v>217</v>
       </c>
       <c r="L38" s="2"/>
       <c r="M38" s="2" t="s">
@@ -8858,8 +8861,8 @@
     </row>
   </sheetData>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:T52">
+    <sortCondition ref="I3:I52"/>
     <sortCondition ref="H3:H52"/>
-    <sortCondition ref="D3:D52"/>
   </sortState>
   <mergeCells count="8">
     <mergeCell ref="A37:A38"/>
@@ -8880,7 +8883,7 @@
   <dimension ref="A1:K38"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F7" sqref="F7"/>
+      <selection activeCell="K2" sqref="K2:K38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -8959,7 +8962,7 @@
       <c r="J2" s="36" t="s">
         <v>219</v>
       </c>
-      <c r="K2" s="36" t="s">
+      <c r="K2" s="2" t="s">
         <v>189</v>
       </c>
     </row>
@@ -8994,7 +8997,7 @@
       <c r="J3" s="36" t="s">
         <v>223</v>
       </c>
-      <c r="K3" s="36" t="s">
+      <c r="K3" s="2" t="s">
         <v>217</v>
       </c>
     </row>
@@ -9029,7 +9032,7 @@
       <c r="J4" s="36" t="s">
         <v>220</v>
       </c>
-      <c r="K4" s="36" t="s">
+      <c r="K4" s="2" t="s">
         <v>189</v>
       </c>
     </row>
@@ -9064,7 +9067,7 @@
       <c r="J5" s="36" t="s">
         <v>220</v>
       </c>
-      <c r="K5" s="36" t="s">
+      <c r="K5" s="2" t="s">
         <v>216</v>
       </c>
     </row>
@@ -9099,7 +9102,7 @@
       <c r="J6" s="36" t="s">
         <v>220</v>
       </c>
-      <c r="K6" s="36" t="s">
+      <c r="K6" s="2" t="s">
         <v>189</v>
       </c>
     </row>
@@ -9134,7 +9137,7 @@
       <c r="J7" s="36" t="s">
         <v>220</v>
       </c>
-      <c r="K7" s="36" t="s">
+      <c r="K7" s="2" t="s">
         <v>217</v>
       </c>
     </row>
@@ -9169,7 +9172,7 @@
       <c r="J8" s="36" t="s">
         <v>220</v>
       </c>
-      <c r="K8" s="36" t="s">
+      <c r="K8" s="2" t="s">
         <v>189</v>
       </c>
     </row>
@@ -9204,8 +9207,8 @@
       <c r="J9" s="36" t="s">
         <v>220</v>
       </c>
-      <c r="K9" s="36" t="s">
-        <v>216</v>
+      <c r="K9" s="2" t="s">
+        <v>189</v>
       </c>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.2">
@@ -9239,7 +9242,7 @@
       <c r="J10" s="36" t="s">
         <v>220</v>
       </c>
-      <c r="K10" s="36" t="s">
+      <c r="K10" s="2" t="s">
         <v>189</v>
       </c>
     </row>
@@ -9274,7 +9277,7 @@
       <c r="J11" s="36" t="s">
         <v>220</v>
       </c>
-      <c r="K11" s="36" t="s">
+      <c r="K11" s="2" t="s">
         <v>189</v>
       </c>
     </row>
@@ -9309,7 +9312,7 @@
       <c r="J12" s="36" t="s">
         <v>220</v>
       </c>
-      <c r="K12" s="36" t="s">
+      <c r="K12" s="2" t="s">
         <v>216</v>
       </c>
     </row>
@@ -9344,7 +9347,7 @@
       <c r="J13" s="36" t="s">
         <v>222</v>
       </c>
-      <c r="K13" s="36" t="s">
+      <c r="K13" s="2" t="s">
         <v>217</v>
       </c>
     </row>
@@ -9379,7 +9382,7 @@
       <c r="J14" s="36" t="s">
         <v>220</v>
       </c>
-      <c r="K14" s="36" t="s">
+      <c r="K14" s="2" t="s">
         <v>217</v>
       </c>
     </row>
@@ -9414,7 +9417,7 @@
       <c r="J15" s="36" t="s">
         <v>220</v>
       </c>
-      <c r="K15" s="36" t="s">
+      <c r="K15" s="2" t="s">
         <v>217</v>
       </c>
     </row>
@@ -9449,7 +9452,7 @@
       <c r="J16" s="33" t="s">
         <v>219</v>
       </c>
-      <c r="K16" s="33" t="s">
+      <c r="K16" s="9" t="s">
         <v>216</v>
       </c>
     </row>
@@ -9484,7 +9487,7 @@
       <c r="J17" s="33" t="s">
         <v>219</v>
       </c>
-      <c r="K17" s="33" t="s">
+      <c r="K17" s="9" t="s">
         <v>216</v>
       </c>
     </row>
@@ -9519,7 +9522,7 @@
       <c r="J18" s="33" t="s">
         <v>219</v>
       </c>
-      <c r="K18" s="33" t="s">
+      <c r="K18" s="9" t="s">
         <v>216</v>
       </c>
     </row>
@@ -9554,7 +9557,7 @@
       <c r="J19" s="33" t="s">
         <v>220</v>
       </c>
-      <c r="K19" s="33" t="s">
+      <c r="K19" s="9" t="s">
         <v>216</v>
       </c>
     </row>
@@ -9589,7 +9592,7 @@
       <c r="J20" s="36" t="s">
         <v>220</v>
       </c>
-      <c r="K20" s="36" t="s">
+      <c r="K20" s="2" t="s">
         <v>216</v>
       </c>
     </row>
@@ -9624,7 +9627,7 @@
       <c r="J21" s="36" t="s">
         <v>220</v>
       </c>
-      <c r="K21" s="36" t="s">
+      <c r="K21" s="2" t="s">
         <v>216</v>
       </c>
     </row>
@@ -9659,7 +9662,7 @@
       <c r="J22" s="36" t="s">
         <v>220</v>
       </c>
-      <c r="K22" s="33" t="s">
+      <c r="K22" s="9" t="s">
         <v>216</v>
       </c>
     </row>
@@ -9694,7 +9697,7 @@
       <c r="J23" s="36" t="s">
         <v>220</v>
       </c>
-      <c r="K23" s="33" t="s">
+      <c r="K23" s="9" t="s">
         <v>216</v>
       </c>
     </row>
@@ -9729,7 +9732,7 @@
       <c r="J24" s="36" t="s">
         <v>222</v>
       </c>
-      <c r="K24" s="36" t="s">
+      <c r="K24" s="2" t="s">
         <v>216</v>
       </c>
     </row>
@@ -9764,7 +9767,7 @@
       <c r="J25" s="36" t="s">
         <v>222</v>
       </c>
-      <c r="K25" s="36" t="s">
+      <c r="K25" s="2" t="s">
         <v>216</v>
       </c>
     </row>
@@ -9799,7 +9802,7 @@
       <c r="J26" s="36" t="s">
         <v>223</v>
       </c>
-      <c r="K26" s="36" t="s">
+      <c r="K26" s="2" t="s">
         <v>217</v>
       </c>
     </row>
@@ -9834,7 +9837,7 @@
       <c r="J27" s="36" t="s">
         <v>223</v>
       </c>
-      <c r="K27" s="36" t="s">
+      <c r="K27" s="2" t="s">
         <v>217</v>
       </c>
     </row>
@@ -9869,7 +9872,7 @@
       <c r="J28" s="36" t="s">
         <v>223</v>
       </c>
-      <c r="K28" s="36" t="s">
+      <c r="K28" s="2" t="s">
         <v>217</v>
       </c>
     </row>
@@ -9904,7 +9907,7 @@
       <c r="J29" s="36" t="s">
         <v>223</v>
       </c>
-      <c r="K29" s="36" t="s">
+      <c r="K29" s="2" t="s">
         <v>217</v>
       </c>
     </row>
@@ -9939,7 +9942,7 @@
       <c r="J30" s="36" t="s">
         <v>223</v>
       </c>
-      <c r="K30" s="36" t="s">
+      <c r="K30" s="2" t="s">
         <v>217</v>
       </c>
     </row>
@@ -9974,7 +9977,7 @@
       <c r="J31" s="36" t="s">
         <v>222</v>
       </c>
-      <c r="K31" s="36" t="s">
+      <c r="K31" s="2" t="s">
         <v>113</v>
       </c>
     </row>
@@ -10009,7 +10012,7 @@
       <c r="J32" s="36" t="s">
         <v>222</v>
       </c>
-      <c r="K32" s="36" t="s">
+      <c r="K32" s="2" t="s">
         <v>189</v>
       </c>
     </row>
@@ -10044,7 +10047,7 @@
       <c r="J33" s="36" t="s">
         <v>222</v>
       </c>
-      <c r="K33" s="36" t="s">
+      <c r="K33" s="2" t="s">
         <v>217</v>
       </c>
     </row>
@@ -10079,7 +10082,7 @@
       <c r="J34" s="36" t="s">
         <v>223</v>
       </c>
-      <c r="K34" s="36" t="s">
+      <c r="K34" s="2" t="s">
         <v>217</v>
       </c>
     </row>
@@ -10114,7 +10117,7 @@
       <c r="J35" s="36" t="s">
         <v>223</v>
       </c>
-      <c r="K35" s="36" t="s">
+      <c r="K35" s="2" t="s">
         <v>189</v>
       </c>
     </row>
@@ -10149,7 +10152,7 @@
       <c r="J36" s="36" t="s">
         <v>223</v>
       </c>
-      <c r="K36" s="36" t="s">
+      <c r="K36" s="2" t="s">
         <v>189</v>
       </c>
     </row>
@@ -10184,7 +10187,7 @@
       <c r="J37" s="36" t="s">
         <v>224</v>
       </c>
-      <c r="K37" s="36" t="s">
+      <c r="K37" s="2" t="s">
         <v>217</v>
       </c>
     </row>
@@ -10219,7 +10222,7 @@
       <c r="J38" s="36" t="s">
         <v>224</v>
       </c>
-      <c r="K38" s="36" t="s">
+      <c r="K38" s="2" t="s">
         <v>217</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Added DEM layer to maps. Can extract elevation data now.
</commit_message>
<xml_diff>
--- a/data/combined_14Clocations-edits.xlsx
+++ b/data/combined_14Clocations-edits.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11028"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11010"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/christopherkiahtipes/Dropbox/Temporary/2023_UGhent_Talk/Mapping_Bantu/data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ckiahtipes/Dropbox/Temporary/2023_UGhent_Talk/Mapping_Bantu/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1D38D6C9-5B8B-3E46-A8D8-AB8F7BFCCE7C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C90D2B30-CEB9-3645-A2CA-02BE061D4EA7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="36700" yWindow="500" windowWidth="28040" windowHeight="17260" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="23160" yWindow="500" windowWidth="28040" windowHeight="17260" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="combined_14Clocations-edits" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1710" uniqueCount="232">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1710" uniqueCount="233">
   <si>
     <t>LON</t>
   </si>
@@ -723,6 +723,9 @@
   </si>
   <si>
     <t>Lebamba et al. 2016; Nguetsop 2013*</t>
+  </si>
+  <si>
+    <t>NYABESSAN</t>
   </si>
 </sst>
 </file>
@@ -1316,7 +1319,7 @@
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="37">
+  <cellXfs count="38">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
@@ -1384,10 +1387,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1836,7 +1842,7 @@
       </c>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A3" s="34" t="s">
+      <c r="A3" s="35" t="s">
         <v>128</v>
       </c>
       <c r="B3" s="2" t="s">
@@ -1942,7 +1948,7 @@
       </c>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A6" s="34" t="s">
+      <c r="A6" s="35" t="s">
         <v>129</v>
       </c>
       <c r="B6" s="2" t="s">
@@ -2012,7 +2018,7 @@
       </c>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A8" s="34" t="s">
+      <c r="A8" s="35" t="s">
         <v>4</v>
       </c>
       <c r="B8" s="2" t="s">
@@ -2082,7 +2088,7 @@
       </c>
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A10" s="34" t="s">
+      <c r="A10" s="35" t="s">
         <v>3</v>
       </c>
       <c r="B10" s="2" t="s">
@@ -2186,7 +2192,7 @@
       </c>
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A13" s="34" t="s">
+      <c r="A13" s="35" t="s">
         <v>130</v>
       </c>
       <c r="B13" s="2" t="s">
@@ -2256,7 +2262,7 @@
       </c>
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A15" s="34" t="s">
+      <c r="A15" s="35" t="s">
         <v>126</v>
       </c>
       <c r="B15" s="2" t="s">
@@ -2292,7 +2298,7 @@
       </c>
     </row>
     <row r="16" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A16" s="35"/>
+      <c r="A16" s="37"/>
       <c r="B16" s="2" t="s">
         <v>25</v>
       </c>
@@ -2834,7 +2840,7 @@
       </c>
     </row>
     <row r="31" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A31" s="34" t="s">
+      <c r="A31" s="35" t="s">
         <v>97</v>
       </c>
       <c r="B31" s="4" t="s">
@@ -2872,7 +2878,7 @@
       </c>
     </row>
     <row r="32" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A32" s="35"/>
+      <c r="A32" s="37"/>
       <c r="B32" s="4" t="s">
         <v>115</v>
       </c>
@@ -2904,7 +2910,7 @@
       </c>
     </row>
     <row r="33" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A33" s="35"/>
+      <c r="A33" s="37"/>
       <c r="B33" s="4" t="s">
         <v>116</v>
       </c>
@@ -2936,7 +2942,7 @@
       </c>
     </row>
     <row r="34" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A34" s="35"/>
+      <c r="A34" s="37"/>
       <c r="B34" s="4" t="s">
         <v>117</v>
       </c>
@@ -3000,7 +3006,7 @@
       </c>
     </row>
     <row r="36" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A36" s="34" t="s">
+      <c r="A36" s="35" t="s">
         <v>121</v>
       </c>
       <c r="B36" s="4" t="s">
@@ -4002,7 +4008,7 @@
       </c>
     </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A3" s="34" t="s">
+      <c r="A3" s="35" t="s">
         <v>128</v>
       </c>
       <c r="B3" s="2" t="s">
@@ -4128,7 +4134,7 @@
       </c>
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A6" s="34" t="s">
+      <c r="A6" s="35" t="s">
         <v>129</v>
       </c>
       <c r="B6" s="2" t="s">
@@ -4210,7 +4216,7 @@
       </c>
     </row>
     <row r="8" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A8" s="34" t="s">
+      <c r="A8" s="35" t="s">
         <v>4</v>
       </c>
       <c r="B8" s="2" t="s">
@@ -4292,7 +4298,7 @@
       </c>
     </row>
     <row r="10" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A10" s="34" t="s">
+      <c r="A10" s="35" t="s">
         <v>3</v>
       </c>
       <c r="B10" s="2" t="s">
@@ -4418,7 +4424,7 @@
       </c>
     </row>
     <row r="13" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A13" s="34" t="s">
+      <c r="A13" s="35" t="s">
         <v>130</v>
       </c>
       <c r="B13" s="2" t="s">
@@ -4500,7 +4506,7 @@
       </c>
     </row>
     <row r="15" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A15" s="34" t="s">
+      <c r="A15" s="35" t="s">
         <v>126</v>
       </c>
       <c r="B15" s="2" t="s">
@@ -4542,7 +4548,7 @@
       </c>
     </row>
     <row r="16" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A16" s="35"/>
+      <c r="A16" s="37"/>
       <c r="B16" s="2" t="s">
         <v>25</v>
       </c>
@@ -4918,7 +4924,7 @@
       </c>
     </row>
     <row r="25" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A25" s="34" t="s">
+      <c r="A25" s="35" t="s">
         <v>97</v>
       </c>
       <c r="B25" s="2" t="s">
@@ -4960,7 +4966,7 @@
       </c>
     </row>
     <row r="26" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A26" s="35"/>
+      <c r="A26" s="37"/>
       <c r="B26" s="2" t="s">
         <v>115</v>
       </c>
@@ -4996,7 +5002,7 @@
       </c>
     </row>
     <row r="27" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A27" s="35"/>
+      <c r="A27" s="37"/>
       <c r="B27" s="2" t="s">
         <v>116</v>
       </c>
@@ -5032,7 +5038,7 @@
       </c>
     </row>
     <row r="28" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A28" s="35"/>
+      <c r="A28" s="37"/>
       <c r="B28" s="2" t="s">
         <v>117</v>
       </c>
@@ -5104,7 +5110,7 @@
       </c>
     </row>
     <row r="30" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A30" s="34" t="s">
+      <c r="A30" s="35" t="s">
         <v>121</v>
       </c>
       <c r="B30" s="2" t="s">
@@ -7361,8 +7367,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B80A1C97-BE26-1B43-924D-147B48F4DDB3}">
   <dimension ref="A1:M38"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="J26" sqref="J26:K26"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A15" sqref="A15:XFD15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -7420,199 +7426,203 @@
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A2" s="12" t="s">
-        <v>132</v>
+        <v>135</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>74</v>
+        <v>80</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>73</v>
+        <v>10</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>189</v>
+        <v>216</v>
       </c>
       <c r="E2" s="5">
-        <v>101</v>
-      </c>
-      <c r="F2" s="5" t="s">
-        <v>41</v>
+        <v>1110</v>
+      </c>
+      <c r="F2" s="5">
+        <v>27416</v>
       </c>
       <c r="G2" s="16">
-        <v>6.4333330000000002</v>
+        <v>13.733333333333301</v>
       </c>
       <c r="H2" s="16">
-        <v>4.55</v>
+        <v>7.31666666666667</v>
       </c>
       <c r="I2" s="2" t="s">
-        <v>75</v>
+        <v>65</v>
       </c>
       <c r="J2" s="2" t="s">
-        <v>180</v>
+        <v>183</v>
       </c>
       <c r="K2" s="2" t="s">
-        <v>219</v>
+        <v>220</v>
       </c>
       <c r="L2" s="2"/>
       <c r="M2" s="2" t="s">
-        <v>154</v>
+        <v>161</v>
       </c>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A3" s="12" t="s">
-        <v>125</v>
+      <c r="A3" s="34" t="s">
+        <v>134</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>106</v>
+        <v>79</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>105</v>
+        <v>15</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>217</v>
+        <v>189</v>
       </c>
       <c r="E3" s="5">
-        <v>156</v>
-      </c>
-      <c r="F3" s="5" t="s">
-        <v>41</v>
+        <v>1160</v>
+      </c>
+      <c r="F3" s="5">
+        <v>27428</v>
       </c>
       <c r="G3" s="16">
-        <v>10.4</v>
+        <v>13.58333</v>
       </c>
       <c r="H3" s="16">
-        <v>2.39</v>
+        <v>7.25</v>
       </c>
       <c r="I3" s="2" t="s">
         <v>65</v>
       </c>
       <c r="J3" s="2" t="s">
-        <v>180</v>
+        <v>183</v>
       </c>
       <c r="K3" s="2" t="s">
-        <v>223</v>
-      </c>
-      <c r="L3" s="2"/>
+        <v>220</v>
+      </c>
+      <c r="L3" s="2">
+        <v>6</v>
+      </c>
       <c r="M3" s="2" t="s">
-        <v>178</v>
+        <v>231</v>
       </c>
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A4" s="34" t="s">
-        <v>130</v>
+        <v>78</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>62</v>
+        <v>27</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>61</v>
+        <v>78</v>
       </c>
       <c r="D4" s="2" t="s">
         <v>189</v>
       </c>
       <c r="E4" s="5">
-        <v>242</v>
+        <v>2015</v>
       </c>
       <c r="F4" s="5" t="s">
         <v>41</v>
       </c>
       <c r="G4" s="16">
-        <v>9.9964650000000006</v>
+        <v>10.348549</v>
       </c>
       <c r="H4" s="16">
-        <v>3.77</v>
+        <v>6.0892730000000004</v>
       </c>
       <c r="I4" s="2" t="s">
         <v>65</v>
       </c>
       <c r="J4" s="2" t="s">
-        <v>180</v>
+        <v>183</v>
       </c>
       <c r="K4" s="2" t="s">
         <v>220</v>
       </c>
       <c r="L4" s="2"/>
       <c r="M4" s="2" t="s">
-        <v>150</v>
+        <v>158</v>
       </c>
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A5" s="36"/>
+      <c r="A5" s="34" t="s">
+        <v>127</v>
+      </c>
       <c r="B5" s="4" t="s">
-        <v>64</v>
+        <v>77</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>63</v>
+        <v>76</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>216</v>
+        <v>189</v>
       </c>
       <c r="E5" s="5">
-        <v>19</v>
+        <v>2273</v>
       </c>
       <c r="F5" s="5">
-        <v>28312</v>
+        <v>23662</v>
       </c>
       <c r="G5" s="16">
-        <v>9.9964650000000006</v>
+        <v>10.240641</v>
       </c>
       <c r="H5" s="16">
-        <v>3.7791410000000001</v>
+        <v>5.9336890000000002</v>
       </c>
       <c r="I5" s="2" t="s">
         <v>65</v>
       </c>
       <c r="J5" s="2" t="s">
-        <v>180</v>
+        <v>183</v>
       </c>
       <c r="K5" s="2" t="s">
         <v>220</v>
       </c>
       <c r="L5" s="2"/>
       <c r="M5" s="2" t="s">
-        <v>149</v>
+        <v>156</v>
       </c>
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A6" s="12" t="s">
-        <v>131</v>
+      <c r="A6" s="34" t="s">
+        <v>133</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>71</v>
+        <v>29</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>70</v>
+        <v>133</v>
       </c>
       <c r="D6" s="2" t="s">
         <v>189</v>
       </c>
-      <c r="E6" s="5" t="s">
-        <v>41</v>
-      </c>
-      <c r="F6" s="5">
-        <v>29066</v>
+      <c r="E6" s="5">
+        <v>1191</v>
+      </c>
+      <c r="F6" s="5" t="s">
+        <v>41</v>
       </c>
       <c r="G6" s="16">
-        <v>9.2689000000000004</v>
+        <v>10.581908</v>
       </c>
       <c r="H6" s="16">
-        <v>4.45</v>
+        <v>5.5660420000000004</v>
       </c>
       <c r="I6" s="2" t="s">
         <v>65</v>
       </c>
       <c r="J6" s="2" t="s">
-        <v>180</v>
+        <v>183</v>
       </c>
       <c r="K6" s="2" t="s">
         <v>220</v>
       </c>
       <c r="L6" s="2"/>
       <c r="M6" s="2" t="s">
-        <v>153</v>
+        <v>155</v>
       </c>
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A7" s="7" t="s">
+      <c r="A7" s="34" t="s">
         <v>110</v>
       </c>
       <c r="B7" s="4" t="s">
@@ -7651,226 +7661,222 @@
       </c>
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A8" s="7" t="s">
-        <v>133</v>
+      <c r="A8" s="34" t="s">
+        <v>131</v>
       </c>
       <c r="B8" s="4" t="s">
-        <v>29</v>
+        <v>71</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>133</v>
+        <v>70</v>
       </c>
       <c r="D8" s="2" t="s">
         <v>189</v>
       </c>
-      <c r="E8" s="5">
-        <v>1191</v>
-      </c>
-      <c r="F8" s="5" t="s">
-        <v>41</v>
+      <c r="E8" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="F8" s="5">
+        <v>29066</v>
       </c>
       <c r="G8" s="16">
-        <v>10.581908</v>
+        <v>9.2689000000000004</v>
       </c>
       <c r="H8" s="16">
-        <v>5.5660420000000004</v>
+        <v>4.45</v>
       </c>
       <c r="I8" s="2" t="s">
         <v>65</v>
       </c>
       <c r="J8" s="2" t="s">
-        <v>183</v>
+        <v>180</v>
       </c>
       <c r="K8" s="2" t="s">
         <v>220</v>
       </c>
       <c r="L8" s="2"/>
       <c r="M8" s="2" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
     </row>
     <row r="9" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A9" s="7" t="s">
-        <v>127</v>
+      <c r="A9" s="35" t="s">
+        <v>130</v>
       </c>
       <c r="B9" s="4" t="s">
-        <v>77</v>
+        <v>64</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>76</v>
+        <v>63</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>189</v>
+        <v>216</v>
       </c>
       <c r="E9" s="5">
-        <v>2273</v>
+        <v>19</v>
       </c>
       <c r="F9" s="5">
-        <v>23662</v>
+        <v>28312</v>
       </c>
       <c r="G9" s="16">
-        <v>10.240641</v>
+        <v>9.9964650000000006</v>
       </c>
       <c r="H9" s="16">
-        <v>5.9336890000000002</v>
+        <v>3.7791410000000001</v>
       </c>
       <c r="I9" s="2" t="s">
         <v>65</v>
       </c>
       <c r="J9" s="2" t="s">
-        <v>183</v>
+        <v>180</v>
       </c>
       <c r="K9" s="2" t="s">
         <v>220</v>
       </c>
       <c r="L9" s="2"/>
       <c r="M9" s="2" t="s">
-        <v>156</v>
+        <v>149</v>
       </c>
     </row>
     <row r="10" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A10" s="7" t="s">
-        <v>78</v>
-      </c>
+      <c r="A10" s="36"/>
       <c r="B10" s="4" t="s">
-        <v>27</v>
+        <v>62</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>78</v>
+        <v>61</v>
       </c>
       <c r="D10" s="2" t="s">
         <v>189</v>
       </c>
       <c r="E10" s="5">
-        <v>2015</v>
+        <v>242</v>
       </c>
       <c r="F10" s="5" t="s">
         <v>41</v>
       </c>
       <c r="G10" s="16">
-        <v>10.348549</v>
+        <v>9.9964650000000006</v>
       </c>
       <c r="H10" s="16">
-        <v>6.0892730000000004</v>
+        <v>3.77</v>
       </c>
       <c r="I10" s="2" t="s">
         <v>65</v>
       </c>
       <c r="J10" s="2" t="s">
-        <v>183</v>
+        <v>180</v>
       </c>
       <c r="K10" s="2" t="s">
         <v>220</v>
       </c>
       <c r="L10" s="2"/>
       <c r="M10" s="2" t="s">
-        <v>158</v>
+        <v>150</v>
       </c>
     </row>
     <row r="11" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A11" s="7" t="s">
-        <v>134</v>
+      <c r="A11" s="12" t="s">
+        <v>125</v>
       </c>
       <c r="B11" s="4" t="s">
-        <v>79</v>
+        <v>232</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>15</v>
+        <v>125</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>189</v>
+        <v>217</v>
       </c>
       <c r="E11" s="5">
-        <v>1160</v>
-      </c>
-      <c r="F11" s="5">
-        <v>27428</v>
+        <v>156</v>
+      </c>
+      <c r="F11" s="5" t="s">
+        <v>41</v>
       </c>
       <c r="G11" s="16">
-        <v>13.58333</v>
+        <v>10.4</v>
       </c>
       <c r="H11" s="16">
-        <v>7.25</v>
+        <v>2.39</v>
       </c>
       <c r="I11" s="2" t="s">
         <v>65</v>
       </c>
       <c r="J11" s="2" t="s">
-        <v>183</v>
+        <v>180</v>
       </c>
       <c r="K11" s="2" t="s">
-        <v>220</v>
-      </c>
-      <c r="L11" s="2">
-        <v>6</v>
-      </c>
+        <v>223</v>
+      </c>
+      <c r="L11" s="2"/>
       <c r="M11" s="2" t="s">
-        <v>231</v>
+        <v>178</v>
       </c>
     </row>
     <row r="12" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A12" s="7" t="s">
-        <v>135</v>
+      <c r="A12" s="12" t="s">
+        <v>122</v>
       </c>
       <c r="B12" s="4" t="s">
-        <v>80</v>
+        <v>92</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>10</v>
+        <v>91</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>216</v>
+        <v>217</v>
       </c>
       <c r="E12" s="5">
-        <v>1110</v>
-      </c>
-      <c r="F12" s="5">
-        <v>27416</v>
+        <v>350</v>
+      </c>
+      <c r="F12" s="5" t="s">
+        <v>41</v>
       </c>
       <c r="G12" s="16">
-        <v>13.733333333333301</v>
+        <v>11.77</v>
       </c>
       <c r="H12" s="16">
-        <v>7.31666666666667</v>
+        <v>-0.72</v>
       </c>
       <c r="I12" s="2" t="s">
-        <v>65</v>
+        <v>169</v>
       </c>
       <c r="J12" s="2" t="s">
-        <v>183</v>
+        <v>180</v>
       </c>
       <c r="K12" s="2" t="s">
-        <v>220</v>
+        <v>222</v>
       </c>
       <c r="L12" s="2"/>
       <c r="M12" s="2" t="s">
-        <v>161</v>
+        <v>173</v>
       </c>
     </row>
     <row r="13" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A13" s="12" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="B13" s="4" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>91</v>
+        <v>93</v>
       </c>
       <c r="D13" s="2" t="s">
         <v>217</v>
       </c>
       <c r="E13" s="5">
-        <v>350</v>
+        <v>20</v>
       </c>
       <c r="F13" s="5" t="s">
         <v>41</v>
       </c>
       <c r="G13" s="16">
-        <v>11.77</v>
+        <v>10.47</v>
       </c>
       <c r="H13" s="16">
-        <v>-0.72</v>
+        <v>-0.2</v>
       </c>
       <c r="I13" s="2" t="s">
         <v>169</v>
@@ -7879,37 +7885,37 @@
         <v>180</v>
       </c>
       <c r="K13" s="2" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
       <c r="L13" s="2"/>
       <c r="M13" s="2" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
     </row>
     <row r="14" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A14" s="12" t="s">
-        <v>123</v>
+        <v>95</v>
       </c>
       <c r="B14" s="4" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>93</v>
+        <v>95</v>
       </c>
       <c r="D14" s="2" t="s">
         <v>217</v>
       </c>
       <c r="E14" s="5">
-        <v>20</v>
+        <v>5</v>
       </c>
       <c r="F14" s="5" t="s">
         <v>41</v>
       </c>
       <c r="G14" s="16">
-        <v>10.47</v>
+        <v>9.35</v>
       </c>
       <c r="H14" s="16">
-        <v>-0.2</v>
+        <v>-0.17</v>
       </c>
       <c r="I14" s="2" t="s">
         <v>169</v>
@@ -7922,46 +7928,46 @@
       </c>
       <c r="L14" s="2"/>
       <c r="M14" s="2" t="s">
-        <v>174</v>
+        <v>179</v>
       </c>
     </row>
     <row r="15" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A15" s="12" t="s">
-        <v>95</v>
+      <c r="A15" s="34" t="s">
+        <v>132</v>
       </c>
       <c r="B15" s="4" t="s">
-        <v>96</v>
+        <v>74</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>95</v>
+        <v>73</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>217</v>
+        <v>189</v>
       </c>
       <c r="E15" s="5">
-        <v>5</v>
+        <v>101</v>
       </c>
       <c r="F15" s="5" t="s">
         <v>41</v>
       </c>
       <c r="G15" s="16">
-        <v>9.35</v>
+        <v>6.4333330000000002</v>
       </c>
       <c r="H15" s="16">
-        <v>-0.17</v>
+        <v>4.55</v>
       </c>
       <c r="I15" s="2" t="s">
-        <v>169</v>
+        <v>75</v>
       </c>
       <c r="J15" s="2" t="s">
         <v>180</v>
       </c>
       <c r="K15" s="2" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="L15" s="2"/>
       <c r="M15" s="2" t="s">
-        <v>179</v>
+        <v>154</v>
       </c>
     </row>
     <row r="16" spans="1:13" x14ac:dyDescent="0.2">
@@ -8004,7 +8010,7 @@
       </c>
     </row>
     <row r="17" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A17" s="34" t="s">
+      <c r="A17" s="35" t="s">
         <v>128</v>
       </c>
       <c r="B17" s="4" t="s">
@@ -8121,7 +8127,7 @@
       </c>
     </row>
     <row r="20" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A20" s="34" t="s">
+      <c r="A20" s="35" t="s">
         <v>4</v>
       </c>
       <c r="B20" s="4" t="s">
@@ -8197,7 +8203,7 @@
       </c>
     </row>
     <row r="22" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A22" s="34" t="s">
+      <c r="A22" s="35" t="s">
         <v>129</v>
       </c>
       <c r="B22" s="4" t="s">
@@ -8273,7 +8279,7 @@
       </c>
     </row>
     <row r="24" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A24" s="34" t="s">
+      <c r="A24" s="35" t="s">
         <v>3</v>
       </c>
       <c r="B24" s="4" t="s">
@@ -8349,32 +8355,32 @@
       </c>
     </row>
     <row r="26" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A26" s="34" t="s">
-        <v>97</v>
+      <c r="A26" s="35" t="s">
+        <v>126</v>
       </c>
       <c r="B26" s="4" t="s">
-        <v>116</v>
+        <v>109</v>
       </c>
       <c r="C26" s="2" t="s">
-        <v>97</v>
+        <v>108</v>
       </c>
       <c r="D26" s="2" t="s">
         <v>217</v>
       </c>
       <c r="E26" s="5">
-        <v>327</v>
+        <v>573</v>
       </c>
       <c r="F26" s="5" t="s">
         <v>41</v>
       </c>
-      <c r="G26" s="16">
-        <v>17.75</v>
+      <c r="G26" s="16" t="s">
+        <v>107</v>
       </c>
       <c r="H26" s="16">
-        <v>1.175</v>
+        <v>3.6635</v>
       </c>
       <c r="I26" s="2" t="s">
-        <v>44</v>
+        <v>72</v>
       </c>
       <c r="J26" s="2" t="s">
         <v>227</v>
@@ -8384,34 +8390,34 @@
       </c>
       <c r="L26" s="2"/>
       <c r="M26" s="2" t="s">
-        <v>228</v>
+        <v>152</v>
       </c>
     </row>
     <row r="27" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A27" s="35"/>
+      <c r="A27" s="37"/>
       <c r="B27" s="4" t="s">
-        <v>115</v>
+        <v>69</v>
       </c>
       <c r="C27" s="2" t="s">
-        <v>97</v>
+        <v>68</v>
       </c>
       <c r="D27" s="2" t="s">
-        <v>217</v>
+        <v>189</v>
       </c>
       <c r="E27" s="5">
-        <v>327</v>
+        <v>448</v>
       </c>
       <c r="F27" s="5" t="s">
         <v>41</v>
       </c>
       <c r="G27" s="16">
-        <v>17.8</v>
+        <v>17.466696413370901</v>
       </c>
       <c r="H27" s="16">
-        <v>1.18</v>
+        <v>3.8333759074349998</v>
       </c>
       <c r="I27" s="2" t="s">
-        <v>44</v>
+        <v>72</v>
       </c>
       <c r="J27" s="2" t="s">
         <v>227</v>
@@ -8421,34 +8427,34 @@
       </c>
       <c r="L27" s="2"/>
       <c r="M27" s="2" t="s">
-        <v>228</v>
+        <v>151</v>
       </c>
     </row>
     <row r="28" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A28" s="35"/>
+      <c r="A28" s="36"/>
       <c r="B28" s="4" t="s">
-        <v>88</v>
+        <v>67</v>
       </c>
       <c r="C28" s="2" t="s">
-        <v>97</v>
+        <v>66</v>
       </c>
       <c r="D28" s="2" t="s">
-        <v>217</v>
+        <v>189</v>
       </c>
       <c r="E28" s="5">
-        <v>327</v>
+        <v>459</v>
       </c>
       <c r="F28" s="5" t="s">
         <v>41</v>
       </c>
       <c r="G28" s="16">
-        <v>17.639900000000001</v>
+        <v>16.952105693051401</v>
       </c>
       <c r="H28" s="16">
-        <v>1.1835</v>
+        <v>3.9759219365907299</v>
       </c>
       <c r="I28" s="2" t="s">
-        <v>44</v>
+        <v>72</v>
       </c>
       <c r="J28" s="2" t="s">
         <v>227</v>
@@ -8458,13 +8464,15 @@
       </c>
       <c r="L28" s="2"/>
       <c r="M28" s="2" t="s">
-        <v>228</v>
+        <v>152</v>
       </c>
     </row>
     <row r="29" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A29" s="35"/>
+      <c r="A29" s="35" t="s">
+        <v>97</v>
+      </c>
       <c r="B29" s="4" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="C29" s="2" t="s">
         <v>97</v>
@@ -8479,10 +8487,10 @@
         <v>41</v>
       </c>
       <c r="G29" s="16">
-        <v>17.7</v>
+        <v>17.75</v>
       </c>
       <c r="H29" s="16">
-        <v>1.1835</v>
+        <v>1.175</v>
       </c>
       <c r="I29" s="2" t="s">
         <v>44</v>
@@ -8499,12 +8507,12 @@
       </c>
     </row>
     <row r="30" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A30" s="36"/>
+      <c r="A30" s="37"/>
       <c r="B30" s="4" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
       <c r="C30" s="2" t="s">
-        <v>119</v>
+        <v>97</v>
       </c>
       <c r="D30" s="2" t="s">
         <v>217</v>
@@ -8516,10 +8524,10 @@
         <v>41</v>
       </c>
       <c r="G30" s="16">
-        <v>17.48</v>
+        <v>17.8</v>
       </c>
       <c r="H30" s="16">
-        <v>1.2</v>
+        <v>1.18</v>
       </c>
       <c r="I30" s="2" t="s">
         <v>44</v>
@@ -8536,29 +8544,27 @@
       </c>
     </row>
     <row r="31" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A31" s="7" t="s">
-        <v>124</v>
-      </c>
-      <c r="B31" s="21" t="s">
-        <v>101</v>
+      <c r="A31" s="37"/>
+      <c r="B31" s="4" t="s">
+        <v>88</v>
       </c>
       <c r="C31" s="2" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="D31" s="2" t="s">
-        <v>113</v>
+        <v>217</v>
       </c>
       <c r="E31" s="5">
-        <v>370</v>
+        <v>327</v>
       </c>
       <c r="F31" s="5" t="s">
         <v>41</v>
       </c>
       <c r="G31" s="16">
-        <v>16.510000000000002</v>
+        <v>17.639900000000001</v>
       </c>
       <c r="H31" s="16">
-        <v>2.16</v>
+        <v>1.1835</v>
       </c>
       <c r="I31" s="2" t="s">
         <v>44</v>
@@ -8567,37 +8573,35 @@
         <v>227</v>
       </c>
       <c r="K31" s="2" t="s">
-        <v>222</v>
+        <v>223</v>
       </c>
       <c r="L31" s="2"/>
       <c r="M31" s="2" t="s">
-        <v>175</v>
+        <v>228</v>
       </c>
     </row>
     <row r="32" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A32" s="7" t="s">
-        <v>148</v>
-      </c>
+      <c r="A32" s="37"/>
       <c r="B32" s="4" t="s">
-        <v>17</v>
+        <v>117</v>
       </c>
       <c r="C32" s="2" t="s">
-        <v>147</v>
+        <v>97</v>
       </c>
       <c r="D32" s="2" t="s">
-        <v>189</v>
+        <v>217</v>
       </c>
       <c r="E32" s="5">
-        <v>396</v>
+        <v>327</v>
       </c>
       <c r="F32" s="5" t="s">
         <v>41</v>
       </c>
       <c r="G32" s="16">
-        <v>16.525130000000001</v>
+        <v>17.7</v>
       </c>
       <c r="H32" s="16">
-        <v>2.1872600000000002</v>
+        <v>1.1835</v>
       </c>
       <c r="I32" s="2" t="s">
         <v>44</v>
@@ -8606,39 +8610,35 @@
         <v>227</v>
       </c>
       <c r="K32" s="2" t="s">
-        <v>222</v>
-      </c>
-      <c r="L32" s="2">
-        <v>3</v>
-      </c>
+        <v>223</v>
+      </c>
+      <c r="L32" s="2"/>
       <c r="M32" s="2" t="s">
-        <v>146</v>
+        <v>228</v>
       </c>
     </row>
     <row r="33" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A33" s="12" t="s">
-        <v>102</v>
-      </c>
+      <c r="A33" s="36"/>
       <c r="B33" s="4" t="s">
-        <v>103</v>
+        <v>118</v>
       </c>
       <c r="C33" s="2" t="s">
-        <v>102</v>
+        <v>119</v>
       </c>
       <c r="D33" s="2" t="s">
         <v>217</v>
       </c>
       <c r="E33" s="5">
-        <v>390</v>
+        <v>327</v>
       </c>
       <c r="F33" s="5" t="s">
         <v>41</v>
       </c>
-      <c r="G33" s="16" t="s">
-        <v>104</v>
+      <c r="G33" s="16">
+        <v>17.48</v>
       </c>
       <c r="H33" s="16">
-        <v>2.2405599999999999</v>
+        <v>1.2</v>
       </c>
       <c r="I33" s="2" t="s">
         <v>44</v>
@@ -8647,128 +8647,134 @@
         <v>227</v>
       </c>
       <c r="K33" s="2" t="s">
-        <v>222</v>
+        <v>223</v>
       </c>
       <c r="L33" s="2"/>
       <c r="M33" s="2" t="s">
-        <v>176</v>
+        <v>228</v>
       </c>
     </row>
     <row r="34" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A34" s="34" t="s">
-        <v>126</v>
-      </c>
-      <c r="B34" s="4" t="s">
-        <v>109</v>
+      <c r="A34" s="7" t="s">
+        <v>124</v>
+      </c>
+      <c r="B34" s="21" t="s">
+        <v>101</v>
       </c>
       <c r="C34" s="2" t="s">
-        <v>108</v>
+        <v>100</v>
       </c>
       <c r="D34" s="2" t="s">
-        <v>217</v>
+        <v>113</v>
       </c>
       <c r="E34" s="5">
-        <v>573</v>
+        <v>370</v>
       </c>
       <c r="F34" s="5" t="s">
         <v>41</v>
       </c>
-      <c r="G34" s="16" t="s">
-        <v>107</v>
+      <c r="G34" s="16">
+        <v>16.510000000000002</v>
       </c>
       <c r="H34" s="16">
-        <v>3.6635</v>
+        <v>2.16</v>
       </c>
       <c r="I34" s="2" t="s">
-        <v>72</v>
+        <v>44</v>
       </c>
       <c r="J34" s="2" t="s">
         <v>227</v>
       </c>
       <c r="K34" s="2" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="L34" s="2"/>
       <c r="M34" s="2" t="s">
-        <v>152</v>
+        <v>175</v>
       </c>
     </row>
     <row r="35" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A35" s="35"/>
+      <c r="A35" s="7" t="s">
+        <v>148</v>
+      </c>
       <c r="B35" s="4" t="s">
-        <v>69</v>
+        <v>17</v>
       </c>
       <c r="C35" s="2" t="s">
-        <v>68</v>
+        <v>147</v>
       </c>
       <c r="D35" s="2" t="s">
         <v>189</v>
       </c>
       <c r="E35" s="5">
-        <v>448</v>
+        <v>396</v>
       </c>
       <c r="F35" s="5" t="s">
         <v>41</v>
       </c>
       <c r="G35" s="16">
-        <v>17.466696413370901</v>
+        <v>16.525130000000001</v>
       </c>
       <c r="H35" s="16">
-        <v>3.8333759074349998</v>
+        <v>2.1872600000000002</v>
       </c>
       <c r="I35" s="2" t="s">
-        <v>72</v>
+        <v>44</v>
       </c>
       <c r="J35" s="2" t="s">
         <v>227</v>
       </c>
       <c r="K35" s="2" t="s">
-        <v>223</v>
-      </c>
-      <c r="L35" s="2"/>
+        <v>222</v>
+      </c>
+      <c r="L35" s="2">
+        <v>3</v>
+      </c>
       <c r="M35" s="2" t="s">
-        <v>151</v>
+        <v>146</v>
       </c>
     </row>
     <row r="36" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A36" s="36"/>
+      <c r="A36" s="12" t="s">
+        <v>102</v>
+      </c>
       <c r="B36" s="4" t="s">
-        <v>67</v>
+        <v>103</v>
       </c>
       <c r="C36" s="2" t="s">
-        <v>66</v>
+        <v>102</v>
       </c>
       <c r="D36" s="2" t="s">
-        <v>189</v>
+        <v>217</v>
       </c>
       <c r="E36" s="5">
-        <v>459</v>
+        <v>390</v>
       </c>
       <c r="F36" s="5" t="s">
         <v>41</v>
       </c>
-      <c r="G36" s="16">
-        <v>16.952105693051401</v>
+      <c r="G36" s="16" t="s">
+        <v>104</v>
       </c>
       <c r="H36" s="16">
-        <v>3.9759219365907299</v>
+        <v>2.2405599999999999</v>
       </c>
       <c r="I36" s="2" t="s">
-        <v>72</v>
+        <v>44</v>
       </c>
       <c r="J36" s="2" t="s">
         <v>227</v>
       </c>
       <c r="K36" s="2" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="L36" s="2"/>
       <c r="M36" s="2" t="s">
-        <v>152</v>
+        <v>176</v>
       </c>
     </row>
     <row r="37" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A37" s="34" t="s">
+      <c r="A37" s="35" t="s">
         <v>121</v>
       </c>
       <c r="B37" s="4" t="s">
@@ -8844,19 +8850,18 @@
       </c>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:T52">
-    <sortCondition ref="I3:I52"/>
-    <sortCondition ref="H3:H52"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:M11">
+    <sortCondition descending="1" ref="H2:H11"/>
   </sortState>
   <mergeCells count="8">
     <mergeCell ref="A37:A38"/>
     <mergeCell ref="A20:A21"/>
-    <mergeCell ref="A4:A5"/>
     <mergeCell ref="A17:A18"/>
     <mergeCell ref="A22:A23"/>
     <mergeCell ref="A24:A25"/>
-    <mergeCell ref="A26:A30"/>
-    <mergeCell ref="A34:A36"/>
+    <mergeCell ref="A29:A33"/>
+    <mergeCell ref="A26:A28"/>
+    <mergeCell ref="A9:A10"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Final drafts of figures for ms submission.
</commit_message>
<xml_diff>
--- a/data/combined_14Clocations-edits.xlsx
+++ b/data/combined_14Clocations-edits.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11010"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11028"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ckiahtipes/Dropbox/Temporary/2023_UGhent_Talk/Mapping_Bantu/data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/christopherkiahtipes/Dropbox/Temporary/2023_UGhent_Talk/Mapping_Bantu/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C90D2B30-CEB9-3645-A2CA-02BE061D4EA7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4FD2B537-C26E-0149-BED7-DE13E9437797}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="23160" yWindow="500" windowWidth="28040" windowHeight="17260" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1360" yWindow="740" windowWidth="28040" windowHeight="17260" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="combined_14Clocations-edits" sheetId="1" r:id="rId1"/>
@@ -1319,7 +1319,7 @@
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="38">
+  <cellXfs count="37">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
@@ -1383,9 +1383,6 @@
     <xf numFmtId="0" fontId="18" fillId="33" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="33" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1754,8 +1751,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:L44"/>
   <sheetViews>
-    <sheetView topLeftCell="A18" workbookViewId="0">
-      <selection activeCell="E31" sqref="E31:E44"/>
+    <sheetView topLeftCell="A23" workbookViewId="0">
+      <selection activeCell="L44" sqref="L44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1842,7 +1839,7 @@
       </c>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A3" s="35" t="s">
+      <c r="A3" s="34" t="s">
         <v>128</v>
       </c>
       <c r="B3" s="2" t="s">
@@ -1878,7 +1875,7 @@
       </c>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A4" s="36"/>
+      <c r="A4" s="35"/>
       <c r="B4" s="2" t="s">
         <v>19</v>
       </c>
@@ -1948,7 +1945,7 @@
       </c>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A6" s="35" t="s">
+      <c r="A6" s="34" t="s">
         <v>129</v>
       </c>
       <c r="B6" s="2" t="s">
@@ -1984,7 +1981,7 @@
       </c>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A7" s="36"/>
+      <c r="A7" s="35"/>
       <c r="B7" s="2" t="s">
         <v>21</v>
       </c>
@@ -2018,7 +2015,7 @@
       </c>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A8" s="35" t="s">
+      <c r="A8" s="34" t="s">
         <v>4</v>
       </c>
       <c r="B8" s="2" t="s">
@@ -2054,7 +2051,7 @@
       </c>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A9" s="36"/>
+      <c r="A9" s="35"/>
       <c r="B9" s="2" t="s">
         <v>34</v>
       </c>
@@ -2088,7 +2085,7 @@
       </c>
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A10" s="35" t="s">
+      <c r="A10" s="34" t="s">
         <v>3</v>
       </c>
       <c r="B10" s="2" t="s">
@@ -2124,7 +2121,7 @@
       </c>
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A11" s="36"/>
+      <c r="A11" s="35"/>
       <c r="B11" s="2" t="s">
         <v>143</v>
       </c>
@@ -2192,7 +2189,7 @@
       </c>
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A13" s="35" t="s">
+      <c r="A13" s="34" t="s">
         <v>130</v>
       </c>
       <c r="B13" s="2" t="s">
@@ -2228,7 +2225,7 @@
       </c>
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A14" s="36"/>
+      <c r="A14" s="35"/>
       <c r="B14" s="2" t="s">
         <v>32</v>
       </c>
@@ -2262,7 +2259,7 @@
       </c>
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A15" s="35" t="s">
+      <c r="A15" s="34" t="s">
         <v>126</v>
       </c>
       <c r="B15" s="2" t="s">
@@ -2298,7 +2295,7 @@
       </c>
     </row>
     <row r="16" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A16" s="37"/>
+      <c r="A16" s="36"/>
       <c r="B16" s="2" t="s">
         <v>25</v>
       </c>
@@ -2332,7 +2329,7 @@
       </c>
     </row>
     <row r="17" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A17" s="36"/>
+      <c r="A17" s="35"/>
       <c r="B17" s="4" t="s">
         <v>109</v>
       </c>
@@ -2840,7 +2837,7 @@
       </c>
     </row>
     <row r="31" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A31" s="35" t="s">
+      <c r="A31" s="34" t="s">
         <v>97</v>
       </c>
       <c r="B31" s="4" t="s">
@@ -2878,7 +2875,7 @@
       </c>
     </row>
     <row r="32" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A32" s="37"/>
+      <c r="A32" s="36"/>
       <c r="B32" s="4" t="s">
         <v>115</v>
       </c>
@@ -2910,7 +2907,7 @@
       </c>
     </row>
     <row r="33" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A33" s="37"/>
+      <c r="A33" s="36"/>
       <c r="B33" s="4" t="s">
         <v>116</v>
       </c>
@@ -2942,7 +2939,7 @@
       </c>
     </row>
     <row r="34" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A34" s="37"/>
+      <c r="A34" s="36"/>
       <c r="B34" s="4" t="s">
         <v>117</v>
       </c>
@@ -2974,7 +2971,7 @@
       </c>
     </row>
     <row r="35" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A35" s="36"/>
+      <c r="A35" s="35"/>
       <c r="B35" s="4" t="s">
         <v>118</v>
       </c>
@@ -3006,7 +3003,7 @@
       </c>
     </row>
     <row r="36" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A36" s="35" t="s">
+      <c r="A36" s="34" t="s">
         <v>121</v>
       </c>
       <c r="B36" s="4" t="s">
@@ -3044,7 +3041,7 @@
       </c>
     </row>
     <row r="37" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A37" s="36"/>
+      <c r="A37" s="35"/>
       <c r="B37" s="4" t="s">
         <v>90</v>
       </c>
@@ -3908,7 +3905,7 @@
   <dimension ref="A1:N38"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:N38"/>
+      <selection activeCell="N38" sqref="N1:N38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -4008,7 +4005,7 @@
       </c>
     </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A3" s="35" t="s">
+      <c r="A3" s="34" t="s">
         <v>128</v>
       </c>
       <c r="B3" s="2" t="s">
@@ -4050,7 +4047,7 @@
       </c>
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A4" s="36"/>
+      <c r="A4" s="35"/>
       <c r="B4" s="2" t="s">
         <v>19</v>
       </c>
@@ -4134,7 +4131,7 @@
       </c>
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A6" s="35" t="s">
+      <c r="A6" s="34" t="s">
         <v>129</v>
       </c>
       <c r="B6" s="2" t="s">
@@ -4176,7 +4173,7 @@
       </c>
     </row>
     <row r="7" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A7" s="36"/>
+      <c r="A7" s="35"/>
       <c r="B7" s="2" t="s">
         <v>21</v>
       </c>
@@ -4216,7 +4213,7 @@
       </c>
     </row>
     <row r="8" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A8" s="35" t="s">
+      <c r="A8" s="34" t="s">
         <v>4</v>
       </c>
       <c r="B8" s="2" t="s">
@@ -4258,7 +4255,7 @@
       </c>
     </row>
     <row r="9" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A9" s="36"/>
+      <c r="A9" s="35"/>
       <c r="B9" s="2" t="s">
         <v>34</v>
       </c>
@@ -4298,7 +4295,7 @@
       </c>
     </row>
     <row r="10" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A10" s="35" t="s">
+      <c r="A10" s="34" t="s">
         <v>3</v>
       </c>
       <c r="B10" s="2" t="s">
@@ -4340,7 +4337,7 @@
       </c>
     </row>
     <row r="11" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A11" s="36"/>
+      <c r="A11" s="35"/>
       <c r="B11" s="2" t="s">
         <v>143</v>
       </c>
@@ -4424,7 +4421,7 @@
       </c>
     </row>
     <row r="13" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A13" s="35" t="s">
+      <c r="A13" s="34" t="s">
         <v>130</v>
       </c>
       <c r="B13" s="2" t="s">
@@ -4466,7 +4463,7 @@
       </c>
     </row>
     <row r="14" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A14" s="36"/>
+      <c r="A14" s="35"/>
       <c r="B14" s="2" t="s">
         <v>32</v>
       </c>
@@ -4506,7 +4503,7 @@
       </c>
     </row>
     <row r="15" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A15" s="35" t="s">
+      <c r="A15" s="34" t="s">
         <v>126</v>
       </c>
       <c r="B15" s="2" t="s">
@@ -4548,7 +4545,7 @@
       </c>
     </row>
     <row r="16" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A16" s="37"/>
+      <c r="A16" s="36"/>
       <c r="B16" s="2" t="s">
         <v>25</v>
       </c>
@@ -4588,7 +4585,7 @@
       </c>
     </row>
     <row r="17" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A17" s="36"/>
+      <c r="A17" s="35"/>
       <c r="B17" s="2" t="s">
         <v>109</v>
       </c>
@@ -4924,7 +4921,7 @@
       </c>
     </row>
     <row r="25" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A25" s="35" t="s">
+      <c r="A25" s="34" t="s">
         <v>97</v>
       </c>
       <c r="B25" s="2" t="s">
@@ -4966,7 +4963,7 @@
       </c>
     </row>
     <row r="26" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A26" s="37"/>
+      <c r="A26" s="36"/>
       <c r="B26" s="2" t="s">
         <v>115</v>
       </c>
@@ -5002,7 +4999,7 @@
       </c>
     </row>
     <row r="27" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A27" s="37"/>
+      <c r="A27" s="36"/>
       <c r="B27" s="2" t="s">
         <v>116</v>
       </c>
@@ -5038,7 +5035,7 @@
       </c>
     </row>
     <row r="28" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A28" s="37"/>
+      <c r="A28" s="36"/>
       <c r="B28" s="2" t="s">
         <v>117</v>
       </c>
@@ -5074,7 +5071,7 @@
       </c>
     </row>
     <row r="29" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A29" s="36"/>
+      <c r="A29" s="35"/>
       <c r="B29" s="2" t="s">
         <v>118</v>
       </c>
@@ -5110,7 +5107,7 @@
       </c>
     </row>
     <row r="30" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A30" s="35" t="s">
+      <c r="A30" s="34" t="s">
         <v>121</v>
       </c>
       <c r="B30" s="2" t="s">
@@ -5152,7 +5149,7 @@
       </c>
     </row>
     <row r="31" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A31" s="36"/>
+      <c r="A31" s="35"/>
       <c r="B31" s="2" t="s">
         <v>90</v>
       </c>
@@ -7368,7 +7365,7 @@
   <dimension ref="A1:M38"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A15" sqref="A15:XFD15"/>
+      <selection activeCell="M1" sqref="M1:M1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -7464,7 +7461,7 @@
       </c>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A3" s="34" t="s">
+      <c r="A3" s="7" t="s">
         <v>134</v>
       </c>
       <c r="B3" s="4" t="s">
@@ -7505,7 +7502,7 @@
       </c>
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A4" s="34" t="s">
+      <c r="A4" s="7" t="s">
         <v>78</v>
       </c>
       <c r="B4" s="4" t="s">
@@ -7544,7 +7541,7 @@
       </c>
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A5" s="34" t="s">
+      <c r="A5" s="7" t="s">
         <v>127</v>
       </c>
       <c r="B5" s="4" t="s">
@@ -7583,7 +7580,7 @@
       </c>
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A6" s="34" t="s">
+      <c r="A6" s="7" t="s">
         <v>133</v>
       </c>
       <c r="B6" s="4" t="s">
@@ -7622,7 +7619,7 @@
       </c>
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A7" s="34" t="s">
+      <c r="A7" s="7" t="s">
         <v>110</v>
       </c>
       <c r="B7" s="4" t="s">
@@ -7661,7 +7658,7 @@
       </c>
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A8" s="34" t="s">
+      <c r="A8" s="7" t="s">
         <v>131</v>
       </c>
       <c r="B8" s="4" t="s">
@@ -7700,7 +7697,7 @@
       </c>
     </row>
     <row r="9" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A9" s="35" t="s">
+      <c r="A9" s="34" t="s">
         <v>130</v>
       </c>
       <c r="B9" s="4" t="s">
@@ -7739,7 +7736,7 @@
       </c>
     </row>
     <row r="10" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A10" s="36"/>
+      <c r="A10" s="35"/>
       <c r="B10" s="4" t="s">
         <v>62</v>
       </c>
@@ -7932,7 +7929,7 @@
       </c>
     </row>
     <row r="15" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A15" s="34" t="s">
+      <c r="A15" s="7" t="s">
         <v>132</v>
       </c>
       <c r="B15" s="4" t="s">
@@ -8010,7 +8007,7 @@
       </c>
     </row>
     <row r="17" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A17" s="35" t="s">
+      <c r="A17" s="34" t="s">
         <v>128</v>
       </c>
       <c r="B17" s="4" t="s">
@@ -8049,7 +8046,7 @@
       </c>
     </row>
     <row r="18" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A18" s="36"/>
+      <c r="A18" s="35"/>
       <c r="B18" s="4" t="s">
         <v>50</v>
       </c>
@@ -8127,7 +8124,7 @@
       </c>
     </row>
     <row r="20" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A20" s="35" t="s">
+      <c r="A20" s="34" t="s">
         <v>4</v>
       </c>
       <c r="B20" s="4" t="s">
@@ -8166,7 +8163,7 @@
       </c>
     </row>
     <row r="21" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A21" s="36"/>
+      <c r="A21" s="35"/>
       <c r="B21" s="4" t="s">
         <v>56</v>
       </c>
@@ -8203,7 +8200,7 @@
       </c>
     </row>
     <row r="22" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A22" s="35" t="s">
+      <c r="A22" s="34" t="s">
         <v>129</v>
       </c>
       <c r="B22" s="4" t="s">
@@ -8242,7 +8239,7 @@
       </c>
     </row>
     <row r="23" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A23" s="36"/>
+      <c r="A23" s="35"/>
       <c r="B23" s="4" t="s">
         <v>53</v>
       </c>
@@ -8279,7 +8276,7 @@
       </c>
     </row>
     <row r="24" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A24" s="35" t="s">
+      <c r="A24" s="34" t="s">
         <v>3</v>
       </c>
       <c r="B24" s="4" t="s">
@@ -8318,7 +8315,7 @@
       </c>
     </row>
     <row r="25" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A25" s="36"/>
+      <c r="A25" s="35"/>
       <c r="B25" s="4" t="s">
         <v>60</v>
       </c>
@@ -8355,7 +8352,7 @@
       </c>
     </row>
     <row r="26" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A26" s="35" t="s">
+      <c r="A26" s="34" t="s">
         <v>126</v>
       </c>
       <c r="B26" s="4" t="s">
@@ -8394,7 +8391,7 @@
       </c>
     </row>
     <row r="27" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A27" s="37"/>
+      <c r="A27" s="36"/>
       <c r="B27" s="4" t="s">
         <v>69</v>
       </c>
@@ -8431,7 +8428,7 @@
       </c>
     </row>
     <row r="28" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A28" s="36"/>
+      <c r="A28" s="35"/>
       <c r="B28" s="4" t="s">
         <v>67</v>
       </c>
@@ -8468,7 +8465,7 @@
       </c>
     </row>
     <row r="29" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A29" s="35" t="s">
+      <c r="A29" s="34" t="s">
         <v>97</v>
       </c>
       <c r="B29" s="4" t="s">
@@ -8507,7 +8504,7 @@
       </c>
     </row>
     <row r="30" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A30" s="37"/>
+      <c r="A30" s="36"/>
       <c r="B30" s="4" t="s">
         <v>115</v>
       </c>
@@ -8544,7 +8541,7 @@
       </c>
     </row>
     <row r="31" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A31" s="37"/>
+      <c r="A31" s="36"/>
       <c r="B31" s="4" t="s">
         <v>88</v>
       </c>
@@ -8581,7 +8578,7 @@
       </c>
     </row>
     <row r="32" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A32" s="37"/>
+      <c r="A32" s="36"/>
       <c r="B32" s="4" t="s">
         <v>117</v>
       </c>
@@ -8618,7 +8615,7 @@
       </c>
     </row>
     <row r="33" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A33" s="36"/>
+      <c r="A33" s="35"/>
       <c r="B33" s="4" t="s">
         <v>118</v>
       </c>
@@ -8774,7 +8771,7 @@
       </c>
     </row>
     <row r="37" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A37" s="35" t="s">
+      <c r="A37" s="34" t="s">
         <v>121</v>
       </c>
       <c r="B37" s="4" t="s">
@@ -8813,7 +8810,7 @@
       </c>
     </row>
     <row r="38" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A38" s="36"/>
+      <c r="A38" s="35"/>
       <c r="B38" s="4" t="s">
         <v>90</v>
       </c>
@@ -8854,6 +8851,7 @@
     <sortCondition descending="1" ref="H2:H11"/>
   </sortState>
   <mergeCells count="8">
+    <mergeCell ref="A9:A10"/>
     <mergeCell ref="A37:A38"/>
     <mergeCell ref="A20:A21"/>
     <mergeCell ref="A17:A18"/>
@@ -8861,7 +8859,6 @@
     <mergeCell ref="A24:A25"/>
     <mergeCell ref="A29:A33"/>
     <mergeCell ref="A26:A28"/>
-    <mergeCell ref="A9:A10"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -8872,7 +8869,7 @@
   <dimension ref="A1:K38"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="K2" sqref="K2:K38"/>
+      <selection sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>